<commit_message>
Changes to specifications from Gowtham
</commit_message>
<xml_diff>
--- a/analysis_specifications/analysis2InputSpecifications.xlsx
+++ b/analysis_specifications/analysis2InputSpecifications.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="14">
   <si>
     <t>a</t>
   </si>
@@ -122,14 +122,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -447,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E194"/>
+  <dimension ref="A1:E175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C127" sqref="C127:C181"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1964,7 +1962,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:5">
       <c r="A113" s="1" t="s">
         <v>8</v>
       </c>
@@ -1976,7 +1974,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:5">
       <c r="A114" s="1" t="s">
         <v>8</v>
       </c>
@@ -1988,7 +1986,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:5">
       <c r="A115" s="1" t="s">
         <v>8</v>
       </c>
@@ -2002,7 +2000,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:5">
       <c r="A116" s="1" t="s">
         <v>8</v>
       </c>
@@ -2014,7 +2012,7 @@
       </c>
       <c r="D116" s="1"/>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:5">
       <c r="A117" s="1" t="s">
         <v>8</v>
       </c>
@@ -2026,7 +2024,7 @@
       </c>
       <c r="D117" s="1"/>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:5">
       <c r="A118" s="1" t="s">
         <v>8</v>
       </c>
@@ -2038,7 +2036,7 @@
       </c>
       <c r="D118" s="1"/>
     </row>
-    <row r="119" spans="1:4">
+    <row r="119" spans="1:5">
       <c r="A119" s="1" t="s">
         <v>8</v>
       </c>
@@ -2050,7 +2048,7 @@
       </c>
       <c r="D119" s="1"/>
     </row>
-    <row r="120" spans="1:4">
+    <row r="120" spans="1:5">
       <c r="A120" s="1" t="s">
         <v>8</v>
       </c>
@@ -2062,7 +2060,7 @@
       </c>
       <c r="D120" s="1"/>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:5">
       <c r="A121" s="1" t="s">
         <v>8</v>
       </c>
@@ -2074,7 +2072,7 @@
       </c>
       <c r="D121" s="1"/>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:5">
       <c r="A122" s="1" t="s">
         <v>8</v>
       </c>
@@ -2086,7 +2084,7 @@
       </c>
       <c r="D122" s="1"/>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:5">
       <c r="A123" s="1" t="s">
         <v>8</v>
       </c>
@@ -2098,7 +2096,7 @@
       </c>
       <c r="D123" s="1"/>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:5">
       <c r="A124" s="1" t="s">
         <v>8</v>
       </c>
@@ -2110,7 +2108,7 @@
       </c>
       <c r="D124" s="1"/>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="1:5">
       <c r="A125" s="1" t="s">
         <v>8</v>
       </c>
@@ -2122,7 +2120,7 @@
       </c>
       <c r="D125" s="1"/>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:5">
       <c r="A126" s="1" t="s">
         <v>8</v>
       </c>
@@ -2134,930 +2132,648 @@
       </c>
       <c r="D126" s="1"/>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:5">
       <c r="A127" t="s">
         <v>13</v>
       </c>
       <c r="B127" t="s">
         <v>0</v>
       </c>
-      <c r="C127" s="9">
+      <c r="C127" s="7">
         <v>723</v>
       </c>
       <c r="D127" s="7">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4">
+        <v>24</v>
+      </c>
+      <c r="E127" s="7"/>
+    </row>
+    <row r="128" spans="1:5">
       <c r="A128" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B128" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C128" s="9">
+      <c r="C128" s="7">
         <v>716</v>
       </c>
       <c r="D128" s="7">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4">
+        <v>707</v>
+      </c>
+      <c r="E128" s="7"/>
+    </row>
+    <row r="129" spans="1:5">
       <c r="A129" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B129" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C129" s="9">
+      <c r="C129" s="7">
         <v>1081</v>
       </c>
       <c r="D129" s="7">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4">
+        <v>347</v>
+      </c>
+      <c r="E129" s="7"/>
+    </row>
+    <row r="130" spans="1:5">
       <c r="A130" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B130" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C130" s="9">
+      <c r="C130" s="7">
         <v>405</v>
       </c>
-      <c r="D130" s="7">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4">
+      <c r="D130" s="6"/>
+      <c r="E130" s="7"/>
+    </row>
+    <row r="131" spans="1:5">
       <c r="A131" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B131" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C131" s="9">
+      <c r="C131" s="7">
         <v>251</v>
       </c>
-      <c r="D131" s="7">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4">
+      <c r="D131" s="6"/>
+      <c r="E131" s="7"/>
+    </row>
+    <row r="132" spans="1:5">
       <c r="A132" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B132" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C132" s="9">
+      <c r="C132" s="7">
         <v>735</v>
       </c>
-      <c r="D132" s="7">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4">
+      <c r="D132" s="6"/>
+      <c r="E132" s="7"/>
+    </row>
+    <row r="133" spans="1:5">
       <c r="A133" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B133" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C133" s="9">
+      <c r="C133" s="7">
         <v>729</v>
       </c>
-      <c r="D133" s="7">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4">
+      <c r="D133" s="6"/>
+      <c r="E133" s="7"/>
+    </row>
+    <row r="134" spans="1:5">
       <c r="A134" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B134" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C134" s="9">
+      <c r="C134" s="7">
         <v>862</v>
       </c>
-      <c r="D134" s="7">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4">
+      <c r="D134" s="6"/>
+      <c r="E134" s="7"/>
+    </row>
+    <row r="135" spans="1:5">
       <c r="A135" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B135" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C135" s="9">
+      <c r="C135" s="7">
         <v>1013</v>
       </c>
-      <c r="D135" s="7">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4">
+      <c r="D135" s="6"/>
+      <c r="E135" s="7"/>
+    </row>
+    <row r="136" spans="1:5">
       <c r="A136" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B136" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C136" s="9">
+      <c r="C136" s="7">
         <v>334</v>
       </c>
-      <c r="D136" s="7">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4">
+      <c r="D136" s="6"/>
+      <c r="E136" s="7"/>
+    </row>
+    <row r="137" spans="1:5">
       <c r="A137" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B137" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C137" s="9">
+      <c r="C137" s="7">
         <v>989</v>
       </c>
-      <c r="D137" s="7">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4">
+      <c r="D137" s="6"/>
+      <c r="E137" s="7"/>
+    </row>
+    <row r="138" spans="1:5">
       <c r="A138" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B138" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C138" s="9">
-        <v>788</v>
-      </c>
-      <c r="D138" s="7">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4">
+      <c r="C138" s="7">
+        <v>923</v>
+      </c>
+      <c r="D138" s="6"/>
+      <c r="E138" s="7"/>
+    </row>
+    <row r="139" spans="1:5">
       <c r="A139" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B139" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C139" s="9">
-        <v>923</v>
-      </c>
-      <c r="D139" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4">
+      <c r="C139" s="7">
+        <v>1027</v>
+      </c>
+      <c r="D139" s="6"/>
+      <c r="E139" s="7"/>
+    </row>
+    <row r="140" spans="1:5">
       <c r="A140" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B140" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C140" s="9">
-        <v>1027</v>
-      </c>
-      <c r="D140" s="7">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4">
+      <c r="C140" s="7">
+        <v>710</v>
+      </c>
+      <c r="D140" s="6"/>
+      <c r="E140" s="7"/>
+    </row>
+    <row r="141" spans="1:5">
       <c r="A141" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B141" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C141" s="9">
-        <v>710</v>
-      </c>
-      <c r="D141" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4">
+      <c r="C141" s="7">
+        <v>1031</v>
+      </c>
+      <c r="D141" s="6"/>
+      <c r="E141" s="7"/>
+    </row>
+    <row r="142" spans="1:5">
       <c r="A142" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B142" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C142" s="9">
-        <v>790</v>
-      </c>
-      <c r="D142" s="7">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4">
+      <c r="C142" s="7">
+        <v>859</v>
+      </c>
+      <c r="D142" s="6"/>
+      <c r="E142" s="7"/>
+    </row>
+    <row r="143" spans="1:5">
       <c r="A143" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B143" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C143" s="9">
-        <v>1031</v>
-      </c>
-      <c r="D143" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4">
+      <c r="C143" s="7">
+        <v>1007</v>
+      </c>
+      <c r="D143" s="6"/>
+      <c r="E143" s="7"/>
+    </row>
+    <row r="144" spans="1:5">
       <c r="A144" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B144" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C144" s="9">
-        <v>859</v>
-      </c>
-      <c r="D144" s="7">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4">
+      <c r="C144" s="7">
+        <v>770</v>
+      </c>
+      <c r="D144" s="6"/>
+      <c r="E144" s="7"/>
+    </row>
+    <row r="145" spans="1:5">
       <c r="A145" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B145" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C145" s="9">
-        <v>1007</v>
-      </c>
-      <c r="D145" s="7">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4">
+      <c r="C145" s="7">
+        <v>667</v>
+      </c>
+      <c r="D145" s="6"/>
+      <c r="E145" s="7"/>
+    </row>
+    <row r="146" spans="1:5">
       <c r="A146" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B146" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C146" s="9">
-        <v>770</v>
-      </c>
-      <c r="D146" s="7">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4">
+      <c r="C146" s="7">
+        <v>934</v>
+      </c>
+      <c r="D146" s="6"/>
+      <c r="E146" s="7"/>
+    </row>
+    <row r="147" spans="1:5">
       <c r="A147" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B147" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C147" s="9">
-        <v>667</v>
-      </c>
-      <c r="D147" s="7">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4">
+      <c r="C147" s="7">
+        <v>1087</v>
+      </c>
+      <c r="D147" s="6"/>
+      <c r="E147" s="7"/>
+    </row>
+    <row r="148" spans="1:5">
       <c r="A148" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B148" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C148" s="9">
-        <v>934</v>
-      </c>
-      <c r="D148" s="7">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4">
+      <c r="C148" s="7">
+        <v>715</v>
+      </c>
+      <c r="D148" s="6"/>
+      <c r="E148" s="7"/>
+    </row>
+    <row r="149" spans="1:5">
       <c r="A149" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B149" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C149" s="9">
-        <v>1087</v>
-      </c>
-      <c r="D149" s="7">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4">
+      <c r="C149" s="7">
+        <v>1083</v>
+      </c>
+      <c r="D149" s="6"/>
+      <c r="E149" s="7"/>
+    </row>
+    <row r="150" spans="1:5">
       <c r="A150" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B150" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C150" s="9">
-        <v>715</v>
-      </c>
-      <c r="D150" s="7">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4">
+      <c r="C150" s="7">
+        <v>745</v>
+      </c>
+      <c r="D150" s="6"/>
+      <c r="E150" s="7"/>
+    </row>
+    <row r="151" spans="1:5">
       <c r="A151" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B151" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C151" s="9">
-        <v>1083</v>
-      </c>
-      <c r="D151" s="7">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4">
+      <c r="C151" s="7">
+        <v>765</v>
+      </c>
+      <c r="D151" s="6"/>
+      <c r="E151" s="7"/>
+    </row>
+    <row r="152" spans="1:5">
       <c r="A152" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B152" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C152" s="9">
-        <v>745</v>
-      </c>
-      <c r="D152" s="7">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4">
+      <c r="C152" s="7">
+        <v>1020</v>
+      </c>
+      <c r="D152" s="6"/>
+      <c r="E152" s="7"/>
+    </row>
+    <row r="153" spans="1:5">
       <c r="A153" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B153" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C153" s="9">
-        <v>765</v>
-      </c>
-      <c r="D153" s="7">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4">
+      <c r="C153" s="7">
+        <v>1029</v>
+      </c>
+      <c r="D153" s="6"/>
+      <c r="E153" s="7"/>
+    </row>
+    <row r="154" spans="1:5">
       <c r="A154" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B154" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C154" s="9">
-        <v>787</v>
-      </c>
-      <c r="D154" s="7">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4">
+      <c r="C154" s="7">
+        <v>1011</v>
+      </c>
+      <c r="D154" s="6"/>
+      <c r="E154" s="7"/>
+    </row>
+    <row r="155" spans="1:5">
       <c r="A155" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B155" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C155" s="9">
-        <v>1020</v>
-      </c>
-      <c r="D155" s="7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4">
+      <c r="C155" s="7">
+        <v>1026</v>
+      </c>
+      <c r="D155" s="6"/>
+      <c r="E155" s="7"/>
+    </row>
+    <row r="156" spans="1:5">
       <c r="A156" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B156" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C156" s="9">
-        <v>1029</v>
-      </c>
-      <c r="D156" s="7">
-        <v>888</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4">
+      <c r="C156" s="7">
+        <v>919</v>
+      </c>
+      <c r="D156" s="6"/>
+      <c r="E156" s="7"/>
+    </row>
+    <row r="157" spans="1:5">
       <c r="A157" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B157" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C157" s="9">
-        <v>1011</v>
-      </c>
-      <c r="D157" s="7">
-        <v>994</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4">
+      <c r="C157" s="7">
+        <v>749</v>
+      </c>
+      <c r="D157" s="6"/>
+      <c r="E157" s="7"/>
+    </row>
+    <row r="158" spans="1:5">
       <c r="A158" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B158" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C158" s="9">
-        <v>791</v>
-      </c>
-      <c r="D158" s="7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4">
+      <c r="C158" s="7">
+        <v>1030</v>
+      </c>
+      <c r="D158" s="6"/>
+      <c r="E158" s="7"/>
+    </row>
+    <row r="159" spans="1:5">
       <c r="A159" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B159" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C159" s="9">
-        <v>1026</v>
-      </c>
-      <c r="D159" s="7">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4">
+      <c r="C159" s="7">
+        <v>748</v>
+      </c>
+      <c r="D159" s="6"/>
+      <c r="E159" s="7"/>
+    </row>
+    <row r="160" spans="1:5">
       <c r="A160" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B160" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C160" s="9">
-        <v>786</v>
-      </c>
-      <c r="D160" s="7">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4">
+      <c r="C160" s="7">
+        <v>744</v>
+      </c>
+      <c r="D160" s="6"/>
+      <c r="E160" s="7"/>
+    </row>
+    <row r="161" spans="1:5">
       <c r="A161" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B161" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C161" s="9">
-        <v>919</v>
-      </c>
-      <c r="D161" s="7">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4">
+      <c r="C161" s="7">
+        <v>1003</v>
+      </c>
+      <c r="D161" s="6"/>
+      <c r="E161" s="7"/>
+    </row>
+    <row r="162" spans="1:5">
       <c r="A162" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B162" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C162" s="9">
-        <v>749</v>
-      </c>
-      <c r="D162" s="7">
-        <v>940</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4">
+      <c r="C162" s="7">
+        <v>43</v>
+      </c>
+      <c r="D162" s="6"/>
+      <c r="E162" s="7"/>
+    </row>
+    <row r="163" spans="1:5">
       <c r="A163" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B163" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C163" s="9">
-        <v>798</v>
-      </c>
-      <c r="D163" s="7">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4">
+      <c r="C163" s="7">
+        <v>858</v>
+      </c>
+      <c r="D163" s="6"/>
+      <c r="E163" s="7"/>
+    </row>
+    <row r="164" spans="1:5">
       <c r="A164" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B164" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C164" s="9">
-        <v>1030</v>
-      </c>
-      <c r="D164" s="7">
-        <v>941</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4">
+      <c r="C164" s="7">
+        <v>766</v>
+      </c>
+      <c r="D164" s="6"/>
+      <c r="E164" s="7"/>
+    </row>
+    <row r="165" spans="1:5">
       <c r="A165" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B165" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C165" s="9">
-        <v>748</v>
-      </c>
-      <c r="D165" s="7">
-        <v>889</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4">
+      <c r="C165" s="7">
+        <v>767</v>
+      </c>
+      <c r="D165" s="6"/>
+      <c r="E165" s="7"/>
+    </row>
+    <row r="166" spans="1:5">
       <c r="A166" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B166" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C166" s="9">
-        <v>744</v>
-      </c>
-      <c r="D166" s="7">
-        <v>997</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4">
+      <c r="C166" s="7">
+        <v>769</v>
+      </c>
+      <c r="D166" s="6"/>
+      <c r="E166" s="7"/>
+    </row>
+    <row r="167" spans="1:5">
       <c r="A167" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B167" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C167" s="9">
-        <v>1003</v>
-      </c>
-      <c r="D167" s="7">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4">
+      <c r="C167" s="7">
+        <v>892</v>
+      </c>
+      <c r="D167" s="6"/>
+      <c r="E167" s="7"/>
+    </row>
+    <row r="168" spans="1:5">
       <c r="A168" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B168" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C168" s="9">
-        <v>43</v>
-      </c>
-      <c r="D168" s="7">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4">
+      <c r="C168" s="7">
+        <v>119</v>
+      </c>
+      <c r="D168" s="6"/>
+      <c r="E168" s="7"/>
+    </row>
+    <row r="169" spans="1:5">
       <c r="A169" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B169" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C169" s="9">
-        <v>858</v>
-      </c>
-      <c r="D169" s="7">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4">
+      <c r="C169" s="7">
+        <v>920</v>
+      </c>
+      <c r="D169" s="6"/>
+      <c r="E169" s="7"/>
+    </row>
+    <row r="170" spans="1:5">
       <c r="A170" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B170" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C170" s="9">
-        <v>766</v>
-      </c>
-      <c r="D170" s="7">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4">
+      <c r="C170" s="7">
+        <v>956</v>
+      </c>
+      <c r="D170" s="6"/>
+      <c r="E170" s="7"/>
+    </row>
+    <row r="171" spans="1:5">
       <c r="A171" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B171" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C171" s="9">
-        <v>767</v>
-      </c>
-      <c r="D171" s="7">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4">
+      <c r="C171" s="7">
+        <v>1009</v>
+      </c>
+      <c r="D171" s="6"/>
+      <c r="E171" s="7"/>
+    </row>
+    <row r="172" spans="1:5">
       <c r="A172" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B172" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C172" s="9">
-        <v>769</v>
-      </c>
-      <c r="D172" s="7">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4">
+      <c r="C172" s="7">
+        <v>30</v>
+      </c>
+      <c r="D172" s="6"/>
+      <c r="E172" s="7"/>
+    </row>
+    <row r="173" spans="1:5">
       <c r="A173" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B173" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C173" s="9">
-        <v>892</v>
-      </c>
-      <c r="D173" s="7">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4">
+      <c r="C173" s="7">
+        <v>957</v>
+      </c>
+      <c r="D173" s="6"/>
+      <c r="E173" s="7"/>
+    </row>
+    <row r="174" spans="1:5">
       <c r="A174" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B174" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C174" s="9">
-        <v>119</v>
-      </c>
-      <c r="D174" s="7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4">
+      <c r="C174" s="7">
+        <v>860</v>
+      </c>
+      <c r="D174" s="6"/>
+      <c r="E174" s="7"/>
+    </row>
+    <row r="175" spans="1:5">
       <c r="A175" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B175" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C175" s="9">
-        <v>920</v>
-      </c>
-      <c r="D175" s="7">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4">
-      <c r="A176" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B176" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C176" s="9">
-        <v>956</v>
-      </c>
-      <c r="D176" s="7">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5">
-      <c r="A177" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B177" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C177" s="9">
-        <v>1009</v>
-      </c>
-      <c r="D177" s="7">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5">
-      <c r="A178" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B178" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C178" s="9">
-        <v>30</v>
-      </c>
-      <c r="D178" s="7">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5">
-      <c r="A179" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B179" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C179" s="9">
-        <v>957</v>
-      </c>
-      <c r="D179" s="7">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5">
-      <c r="A180" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B180" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C180" s="9">
-        <v>860</v>
-      </c>
-      <c r="D180" s="7">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5">
-      <c r="A181" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B181" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C181" s="9">
+      <c r="C175" s="7">
         <v>1028</v>
       </c>
-      <c r="D181" s="7">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5">
-      <c r="A182" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B182" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C182" s="5"/>
-      <c r="D182" s="7">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5">
-      <c r="A183" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B183" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C183" s="5"/>
-      <c r="D183" s="7">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5">
-      <c r="A184" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B184" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C184" s="5"/>
-      <c r="D184" s="7">
-        <v>953</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5">
-      <c r="A185" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B185" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C185" s="5"/>
-      <c r="D185" s="7">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="186" spans="1:5">
-      <c r="A186" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B186" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C186" s="5"/>
-      <c r="D186" s="7">
-        <v>954</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5">
-      <c r="A187" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B187" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C187" s="5"/>
-      <c r="D187" s="7">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5">
-      <c r="A188" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B188" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D188" s="7">
-        <v>1006</v>
-      </c>
-      <c r="E188" s="6"/>
-    </row>
-    <row r="189" spans="1:5">
-      <c r="A189" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B189" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D189" s="8">
-        <v>24</v>
-      </c>
-      <c r="E189" s="6"/>
-    </row>
-    <row r="190" spans="1:5">
-      <c r="A190" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B190" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D190" s="8">
-        <v>257</v>
-      </c>
-      <c r="E190" s="6"/>
-    </row>
-    <row r="191" spans="1:5">
-      <c r="A191" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B191" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D191" s="8">
-        <v>325</v>
-      </c>
-      <c r="E191" s="6"/>
-    </row>
-    <row r="192" spans="1:5">
-      <c r="A192" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B192" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D192" s="8">
-        <v>346</v>
-      </c>
-      <c r="E192" s="6"/>
-    </row>
-    <row r="193" spans="1:5">
-      <c r="A193" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B193" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D193" s="8">
-        <v>347</v>
-      </c>
-      <c r="E193" s="6"/>
-    </row>
-    <row r="194" spans="1:5">
-      <c r="A194" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B194" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D194" s="8">
-        <v>707</v>
-      </c>
+      <c r="D175" s="6"/>
+      <c r="E175" s="7"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:D43">

</xml_diff>

<commit_message>
Remove cohort on mortality from azza, and ischemic stroke from Evan
</commit_message>
<xml_diff>
--- a/analysis_specifications/analysis2InputSpecifications.xlsx
+++ b/analysis_specifications/analysis2InputSpecifications.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Sheet1!$A$1:$D$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$174</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="14">
   <si>
     <t>a</t>
   </si>
@@ -445,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E175"/>
+  <dimension ref="A1:E174"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="D115" sqref="D115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1074,15 +1074,15 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C45" s="1">
-        <v>862</v>
-      </c>
-      <c r="D45" s="1">
+        <v>818</v>
+      </c>
+      <c r="D45" s="4">
         <v>25</v>
       </c>
     </row>
@@ -1093,8 +1093,8 @@
       <c r="B46" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C46" s="1">
-        <v>818</v>
+      <c r="C46" s="4">
+        <v>824</v>
       </c>
       <c r="D46" s="4">
         <v>25</v>
@@ -1107,8 +1107,8 @@
       <c r="B47" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C47" s="4">
-        <v>824</v>
+      <c r="C47" s="1">
+        <v>829</v>
       </c>
       <c r="D47" s="4">
         <v>25</v>
@@ -1122,7 +1122,7 @@
         <v>0</v>
       </c>
       <c r="C48" s="1">
-        <v>829</v>
+        <v>833</v>
       </c>
       <c r="D48" s="4">
         <v>25</v>
@@ -1136,7 +1136,7 @@
         <v>0</v>
       </c>
       <c r="C49" s="1">
-        <v>833</v>
+        <v>838</v>
       </c>
       <c r="D49" s="4">
         <v>25</v>
@@ -1150,7 +1150,7 @@
         <v>0</v>
       </c>
       <c r="C50" s="1">
-        <v>838</v>
+        <v>842</v>
       </c>
       <c r="D50" s="4">
         <v>25</v>
@@ -1161,10 +1161,10 @@
         <v>7</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C51" s="1">
-        <v>842</v>
+        <v>812</v>
       </c>
       <c r="D51" s="4">
         <v>25</v>
@@ -1178,7 +1178,7 @@
         <v>1</v>
       </c>
       <c r="C52" s="1">
-        <v>812</v>
+        <v>821</v>
       </c>
       <c r="D52" s="4">
         <v>25</v>
@@ -1192,7 +1192,7 @@
         <v>1</v>
       </c>
       <c r="C53" s="1">
-        <v>821</v>
+        <v>832</v>
       </c>
       <c r="D53" s="4">
         <v>25</v>
@@ -1206,7 +1206,7 @@
         <v>1</v>
       </c>
       <c r="C54" s="1">
-        <v>832</v>
+        <v>836</v>
       </c>
       <c r="D54" s="4">
         <v>25</v>
@@ -1220,7 +1220,7 @@
         <v>1</v>
       </c>
       <c r="C55" s="1">
-        <v>836</v>
+        <v>839</v>
       </c>
       <c r="D55" s="4">
         <v>25</v>
@@ -1234,7 +1234,7 @@
         <v>1</v>
       </c>
       <c r="C56" s="1">
-        <v>839</v>
+        <v>848</v>
       </c>
       <c r="D56" s="4">
         <v>25</v>
@@ -1245,10 +1245,10 @@
         <v>7</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C57" s="1">
-        <v>848</v>
+        <v>823</v>
       </c>
       <c r="D57" s="4">
         <v>25</v>
@@ -1262,7 +1262,7 @@
         <v>2</v>
       </c>
       <c r="C58" s="1">
-        <v>823</v>
+        <v>831</v>
       </c>
       <c r="D58" s="4">
         <v>25</v>
@@ -1276,7 +1276,7 @@
         <v>2</v>
       </c>
       <c r="C59" s="1">
-        <v>831</v>
+        <v>835</v>
       </c>
       <c r="D59" s="4">
         <v>25</v>
@@ -1290,7 +1290,7 @@
         <v>2</v>
       </c>
       <c r="C60" s="1">
-        <v>835</v>
+        <v>840</v>
       </c>
       <c r="D60" s="4">
         <v>25</v>
@@ -1304,7 +1304,7 @@
         <v>2</v>
       </c>
       <c r="C61" s="1">
-        <v>840</v>
+        <v>843</v>
       </c>
       <c r="D61" s="4">
         <v>25</v>
@@ -1318,7 +1318,7 @@
         <v>2</v>
       </c>
       <c r="C62" s="1">
-        <v>843</v>
+        <v>820</v>
       </c>
       <c r="D62" s="4">
         <v>25</v>
@@ -1329,10 +1329,10 @@
         <v>7</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C63" s="1">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="D63" s="4">
         <v>25</v>
@@ -1346,10 +1346,10 @@
         <v>3</v>
       </c>
       <c r="C64" s="1">
-        <v>819</v>
+        <v>822</v>
       </c>
       <c r="D64" s="4">
-        <v>25</v>
+        <v>811</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1360,10 +1360,10 @@
         <v>3</v>
       </c>
       <c r="C65" s="1">
-        <v>822</v>
+        <v>834</v>
       </c>
       <c r="D65" s="4">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1374,10 +1374,10 @@
         <v>3</v>
       </c>
       <c r="C66" s="1">
-        <v>834</v>
+        <v>841</v>
       </c>
       <c r="D66" s="4">
-        <v>810</v>
+        <v>854</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1388,10 +1388,10 @@
         <v>3</v>
       </c>
       <c r="C67" s="1">
-        <v>841</v>
+        <v>830</v>
       </c>
       <c r="D67" s="4">
-        <v>854</v>
+        <v>855</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1401,11 +1401,11 @@
       <c r="B68" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C68" s="1">
-        <v>830</v>
+      <c r="C68" s="4">
+        <v>845</v>
       </c>
       <c r="D68" s="4">
-        <v>855</v>
+        <v>797</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -1415,11 +1415,9 @@
       <c r="B69" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C69" s="4">
-        <v>845</v>
-      </c>
+      <c r="C69" s="1"/>
       <c r="D69" s="4">
-        <v>797</v>
+        <v>795</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1431,7 +1429,7 @@
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="4">
-        <v>795</v>
+        <v>804</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1443,7 +1441,7 @@
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="4">
-        <v>804</v>
+        <v>805</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1455,7 +1453,7 @@
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="4">
-        <v>805</v>
+        <v>850</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1467,7 +1465,7 @@
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="4">
-        <v>850</v>
+        <v>851</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1479,7 +1477,7 @@
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="4">
-        <v>851</v>
+        <v>809</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -1491,7 +1489,7 @@
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="4">
-        <v>809</v>
+        <v>852</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1503,7 +1501,7 @@
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="4">
-        <v>852</v>
+        <v>806</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -1515,7 +1513,7 @@
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="4">
-        <v>806</v>
+        <v>411</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -1527,7 +1525,7 @@
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="4">
-        <v>411</v>
+        <v>463</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -1539,7 +1537,7 @@
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="4">
-        <v>463</v>
+        <v>19</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1551,7 +1549,7 @@
       </c>
       <c r="C80" s="1"/>
       <c r="D80" s="4">
-        <v>19</v>
+        <v>507</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -1563,7 +1561,7 @@
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="4">
-        <v>507</v>
+        <v>765</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -1575,7 +1573,7 @@
       </c>
       <c r="C82" s="1"/>
       <c r="D82" s="4">
-        <v>765</v>
+        <v>766</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1587,7 +1585,7 @@
       </c>
       <c r="C83" s="1"/>
       <c r="D83" s="4">
-        <v>766</v>
+        <v>934</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -1599,7 +1597,7 @@
       </c>
       <c r="C84" s="1"/>
       <c r="D84" s="4">
-        <v>934</v>
+        <v>938</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -1611,7 +1609,7 @@
       </c>
       <c r="C85" s="1"/>
       <c r="D85" s="4">
-        <v>938</v>
+        <v>513</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -1623,7 +1621,7 @@
       </c>
       <c r="C86" s="1"/>
       <c r="D86" s="4">
-        <v>513</v>
+        <v>405</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -1635,7 +1633,7 @@
       </c>
       <c r="C87" s="1"/>
       <c r="D87" s="4">
-        <v>405</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -1647,7 +1645,7 @@
       </c>
       <c r="C88" s="1"/>
       <c r="D88" s="4">
-        <v>1081</v>
+        <v>362</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -1659,7 +1657,7 @@
       </c>
       <c r="C89" s="1"/>
       <c r="D89" s="4">
-        <v>362</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -1671,7 +1669,7 @@
       </c>
       <c r="C90" s="1"/>
       <c r="D90" s="4">
-        <v>1088</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -1683,7 +1681,7 @@
       </c>
       <c r="C91" s="1"/>
       <c r="D91" s="4">
-        <v>1090</v>
+        <v>808</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -1695,7 +1693,7 @@
       </c>
       <c r="C92" s="1"/>
       <c r="D92" s="4">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -1707,7 +1705,7 @@
       </c>
       <c r="C93" s="1"/>
       <c r="D93" s="4">
-        <v>807</v>
+        <v>410</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -1719,7 +1717,7 @@
       </c>
       <c r="C94" s="1"/>
       <c r="D94" s="4">
-        <v>410</v>
+        <v>861</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -1731,19 +1729,21 @@
       </c>
       <c r="C95" s="1"/>
       <c r="D95" s="4">
-        <v>861</v>
+        <v>803</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C96" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="C96" s="1">
+        <v>865</v>
+      </c>
       <c r="D96" s="4">
-        <v>803</v>
+        <v>965</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -1754,10 +1754,10 @@
         <v>0</v>
       </c>
       <c r="C97" s="1">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="D97" s="4">
-        <v>965</v>
+        <v>967</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -1768,10 +1768,10 @@
         <v>0</v>
       </c>
       <c r="C98" s="1">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="D98" s="4">
-        <v>967</v>
+        <v>970</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -1782,10 +1782,10 @@
         <v>0</v>
       </c>
       <c r="C99" s="1">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="D99" s="4">
-        <v>970</v>
+        <v>938</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -1796,10 +1796,10 @@
         <v>0</v>
       </c>
       <c r="C100" s="1">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="D100" s="4">
-        <v>938</v>
+        <v>934</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -1810,10 +1810,10 @@
         <v>0</v>
       </c>
       <c r="C101" s="1">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="D101" s="4">
-        <v>934</v>
+        <v>513</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -1824,10 +1824,10 @@
         <v>0</v>
       </c>
       <c r="C102" s="1">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="D102" s="4">
-        <v>513</v>
+        <v>405</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -1838,10 +1838,10 @@
         <v>0</v>
       </c>
       <c r="C103" s="1">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="D103" s="4">
-        <v>405</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -1852,10 +1852,10 @@
         <v>0</v>
       </c>
       <c r="C104" s="1">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="D104" s="4">
-        <v>1081</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -1866,10 +1866,10 @@
         <v>0</v>
       </c>
       <c r="C105" s="1">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="D105" s="4">
-        <v>1088</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -1880,10 +1880,10 @@
         <v>0</v>
       </c>
       <c r="C106" s="1">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="D106" s="4">
-        <v>1090</v>
+        <v>19</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -1894,10 +1894,10 @@
         <v>0</v>
       </c>
       <c r="C107" s="1">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="D107" s="4">
-        <v>19</v>
+        <v>507</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -1907,11 +1907,9 @@
       <c r="B108" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C108" s="1">
-        <v>876</v>
-      </c>
+      <c r="C108" s="1"/>
       <c r="D108" s="4">
-        <v>507</v>
+        <v>410</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -1923,7 +1921,7 @@
       </c>
       <c r="C109" s="1"/>
       <c r="D109" s="4">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -1935,7 +1933,7 @@
       </c>
       <c r="C110" s="1"/>
       <c r="D110" s="4">
-        <v>411</v>
+        <v>463</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -1947,7 +1945,7 @@
       </c>
       <c r="C111" s="1"/>
       <c r="D111" s="4">
-        <v>463</v>
+        <v>362</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -1959,7 +1957,7 @@
       </c>
       <c r="C112" s="1"/>
       <c r="D112" s="4">
-        <v>362</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -1971,7 +1969,7 @@
       </c>
       <c r="C113" s="1"/>
       <c r="D113" s="4">
-        <v>1104</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -1979,11 +1977,13 @@
         <v>8</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C114" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="C114" s="1">
+        <v>1106</v>
+      </c>
       <c r="D114" s="4">
-        <v>1105</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -1994,10 +1994,10 @@
         <v>1</v>
       </c>
       <c r="C115" s="1">
-        <v>1106</v>
-      </c>
-      <c r="D115" s="4">
-        <v>1081</v>
+        <v>1103</v>
+      </c>
+      <c r="D115" s="1">
+        <v>944</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -2008,7 +2008,7 @@
         <v>1</v>
       </c>
       <c r="C116" s="1">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="D116" s="1"/>
     </row>
@@ -2020,7 +2020,7 @@
         <v>1</v>
       </c>
       <c r="C117" s="1">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="D117" s="1"/>
     </row>
@@ -2032,7 +2032,7 @@
         <v>1</v>
       </c>
       <c r="C118" s="1">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="D118" s="1"/>
     </row>
@@ -2044,7 +2044,7 @@
         <v>1</v>
       </c>
       <c r="C119" s="1">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="D119" s="1"/>
     </row>
@@ -2056,7 +2056,7 @@
         <v>1</v>
       </c>
       <c r="C120" s="1">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="D120" s="1"/>
     </row>
@@ -2068,7 +2068,7 @@
         <v>1</v>
       </c>
       <c r="C121" s="1">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="D121" s="1"/>
     </row>
@@ -2080,7 +2080,7 @@
         <v>1</v>
       </c>
       <c r="C122" s="1">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="D122" s="1"/>
     </row>
@@ -2092,7 +2092,7 @@
         <v>1</v>
       </c>
       <c r="C123" s="1">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="D123" s="1"/>
     </row>
@@ -2104,7 +2104,7 @@
         <v>1</v>
       </c>
       <c r="C124" s="1">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="D124" s="1"/>
     </row>
@@ -2116,34 +2116,37 @@
         <v>1</v>
       </c>
       <c r="C125" s="1">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="D125" s="1"/>
     </row>
     <row r="126" spans="1:5">
-      <c r="A126" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C126" s="1">
-        <v>1093</v>
-      </c>
-      <c r="D126" s="1"/>
+      <c r="A126" t="s">
+        <v>13</v>
+      </c>
+      <c r="B126" t="s">
+        <v>0</v>
+      </c>
+      <c r="C126" s="7">
+        <v>723</v>
+      </c>
+      <c r="D126" s="7">
+        <v>24</v>
+      </c>
+      <c r="E126" s="7"/>
     </row>
     <row r="127" spans="1:5">
-      <c r="A127" t="s">
-        <v>13</v>
-      </c>
-      <c r="B127" t="s">
+      <c r="A127" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B127" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C127" s="7">
-        <v>723</v>
+        <v>716</v>
       </c>
       <c r="D127" s="7">
-        <v>24</v>
+        <v>707</v>
       </c>
       <c r="E127" s="7"/>
     </row>
@@ -2155,10 +2158,10 @@
         <v>0</v>
       </c>
       <c r="C128" s="7">
-        <v>716</v>
+        <v>1081</v>
       </c>
       <c r="D128" s="7">
-        <v>707</v>
+        <v>347</v>
       </c>
       <c r="E128" s="7"/>
     </row>
@@ -2170,11 +2173,9 @@
         <v>0</v>
       </c>
       <c r="C129" s="7">
-        <v>1081</v>
-      </c>
-      <c r="D129" s="7">
-        <v>347</v>
-      </c>
+        <v>405</v>
+      </c>
+      <c r="D129" s="6"/>
       <c r="E129" s="7"/>
     </row>
     <row r="130" spans="1:5">
@@ -2185,7 +2186,7 @@
         <v>0</v>
       </c>
       <c r="C130" s="7">
-        <v>405</v>
+        <v>251</v>
       </c>
       <c r="D130" s="6"/>
       <c r="E130" s="7"/>
@@ -2198,7 +2199,7 @@
         <v>0</v>
       </c>
       <c r="C131" s="7">
-        <v>251</v>
+        <v>735</v>
       </c>
       <c r="D131" s="6"/>
       <c r="E131" s="7"/>
@@ -2211,7 +2212,7 @@
         <v>0</v>
       </c>
       <c r="C132" s="7">
-        <v>735</v>
+        <v>729</v>
       </c>
       <c r="D132" s="6"/>
       <c r="E132" s="7"/>
@@ -2224,7 +2225,7 @@
         <v>0</v>
       </c>
       <c r="C133" s="7">
-        <v>729</v>
+        <v>862</v>
       </c>
       <c r="D133" s="6"/>
       <c r="E133" s="7"/>
@@ -2237,7 +2238,7 @@
         <v>0</v>
       </c>
       <c r="C134" s="7">
-        <v>862</v>
+        <v>1013</v>
       </c>
       <c r="D134" s="6"/>
       <c r="E134" s="7"/>
@@ -2250,7 +2251,7 @@
         <v>0</v>
       </c>
       <c r="C135" s="7">
-        <v>1013</v>
+        <v>334</v>
       </c>
       <c r="D135" s="6"/>
       <c r="E135" s="7"/>
@@ -2263,7 +2264,7 @@
         <v>0</v>
       </c>
       <c r="C136" s="7">
-        <v>334</v>
+        <v>989</v>
       </c>
       <c r="D136" s="6"/>
       <c r="E136" s="7"/>
@@ -2276,7 +2277,7 @@
         <v>0</v>
       </c>
       <c r="C137" s="7">
-        <v>989</v>
+        <v>923</v>
       </c>
       <c r="D137" s="6"/>
       <c r="E137" s="7"/>
@@ -2289,7 +2290,7 @@
         <v>0</v>
       </c>
       <c r="C138" s="7">
-        <v>923</v>
+        <v>1027</v>
       </c>
       <c r="D138" s="6"/>
       <c r="E138" s="7"/>
@@ -2302,7 +2303,7 @@
         <v>0</v>
       </c>
       <c r="C139" s="7">
-        <v>1027</v>
+        <v>710</v>
       </c>
       <c r="D139" s="6"/>
       <c r="E139" s="7"/>
@@ -2315,7 +2316,7 @@
         <v>0</v>
       </c>
       <c r="C140" s="7">
-        <v>710</v>
+        <v>1031</v>
       </c>
       <c r="D140" s="6"/>
       <c r="E140" s="7"/>
@@ -2328,7 +2329,7 @@
         <v>0</v>
       </c>
       <c r="C141" s="7">
-        <v>1031</v>
+        <v>859</v>
       </c>
       <c r="D141" s="6"/>
       <c r="E141" s="7"/>
@@ -2341,7 +2342,7 @@
         <v>0</v>
       </c>
       <c r="C142" s="7">
-        <v>859</v>
+        <v>1007</v>
       </c>
       <c r="D142" s="6"/>
       <c r="E142" s="7"/>
@@ -2354,7 +2355,7 @@
         <v>0</v>
       </c>
       <c r="C143" s="7">
-        <v>1007</v>
+        <v>770</v>
       </c>
       <c r="D143" s="6"/>
       <c r="E143" s="7"/>
@@ -2367,7 +2368,7 @@
         <v>0</v>
       </c>
       <c r="C144" s="7">
-        <v>770</v>
+        <v>667</v>
       </c>
       <c r="D144" s="6"/>
       <c r="E144" s="7"/>
@@ -2380,7 +2381,7 @@
         <v>0</v>
       </c>
       <c r="C145" s="7">
-        <v>667</v>
+        <v>934</v>
       </c>
       <c r="D145" s="6"/>
       <c r="E145" s="7"/>
@@ -2393,7 +2394,7 @@
         <v>0</v>
       </c>
       <c r="C146" s="7">
-        <v>934</v>
+        <v>1087</v>
       </c>
       <c r="D146" s="6"/>
       <c r="E146" s="7"/>
@@ -2406,7 +2407,7 @@
         <v>0</v>
       </c>
       <c r="C147" s="7">
-        <v>1087</v>
+        <v>715</v>
       </c>
       <c r="D147" s="6"/>
       <c r="E147" s="7"/>
@@ -2419,7 +2420,7 @@
         <v>0</v>
       </c>
       <c r="C148" s="7">
-        <v>715</v>
+        <v>1083</v>
       </c>
       <c r="D148" s="6"/>
       <c r="E148" s="7"/>
@@ -2432,7 +2433,7 @@
         <v>0</v>
       </c>
       <c r="C149" s="7">
-        <v>1083</v>
+        <v>745</v>
       </c>
       <c r="D149" s="6"/>
       <c r="E149" s="7"/>
@@ -2445,7 +2446,7 @@
         <v>0</v>
       </c>
       <c r="C150" s="7">
-        <v>745</v>
+        <v>765</v>
       </c>
       <c r="D150" s="6"/>
       <c r="E150" s="7"/>
@@ -2458,7 +2459,7 @@
         <v>0</v>
       </c>
       <c r="C151" s="7">
-        <v>765</v>
+        <v>1020</v>
       </c>
       <c r="D151" s="6"/>
       <c r="E151" s="7"/>
@@ -2471,7 +2472,7 @@
         <v>0</v>
       </c>
       <c r="C152" s="7">
-        <v>1020</v>
+        <v>1029</v>
       </c>
       <c r="D152" s="6"/>
       <c r="E152" s="7"/>
@@ -2484,7 +2485,7 @@
         <v>0</v>
       </c>
       <c r="C153" s="7">
-        <v>1029</v>
+        <v>1011</v>
       </c>
       <c r="D153" s="6"/>
       <c r="E153" s="7"/>
@@ -2497,7 +2498,7 @@
         <v>0</v>
       </c>
       <c r="C154" s="7">
-        <v>1011</v>
+        <v>1026</v>
       </c>
       <c r="D154" s="6"/>
       <c r="E154" s="7"/>
@@ -2510,7 +2511,7 @@
         <v>0</v>
       </c>
       <c r="C155" s="7">
-        <v>1026</v>
+        <v>919</v>
       </c>
       <c r="D155" s="6"/>
       <c r="E155" s="7"/>
@@ -2523,7 +2524,7 @@
         <v>0</v>
       </c>
       <c r="C156" s="7">
-        <v>919</v>
+        <v>749</v>
       </c>
       <c r="D156" s="6"/>
       <c r="E156" s="7"/>
@@ -2536,7 +2537,7 @@
         <v>0</v>
       </c>
       <c r="C157" s="7">
-        <v>749</v>
+        <v>1030</v>
       </c>
       <c r="D157" s="6"/>
       <c r="E157" s="7"/>
@@ -2549,7 +2550,7 @@
         <v>0</v>
       </c>
       <c r="C158" s="7">
-        <v>1030</v>
+        <v>748</v>
       </c>
       <c r="D158" s="6"/>
       <c r="E158" s="7"/>
@@ -2562,7 +2563,7 @@
         <v>0</v>
       </c>
       <c r="C159" s="7">
-        <v>748</v>
+        <v>744</v>
       </c>
       <c r="D159" s="6"/>
       <c r="E159" s="7"/>
@@ -2575,7 +2576,7 @@
         <v>0</v>
       </c>
       <c r="C160" s="7">
-        <v>744</v>
+        <v>1003</v>
       </c>
       <c r="D160" s="6"/>
       <c r="E160" s="7"/>
@@ -2588,7 +2589,7 @@
         <v>0</v>
       </c>
       <c r="C161" s="7">
-        <v>1003</v>
+        <v>43</v>
       </c>
       <c r="D161" s="6"/>
       <c r="E161" s="7"/>
@@ -2601,7 +2602,7 @@
         <v>0</v>
       </c>
       <c r="C162" s="7">
-        <v>43</v>
+        <v>858</v>
       </c>
       <c r="D162" s="6"/>
       <c r="E162" s="7"/>
@@ -2614,7 +2615,7 @@
         <v>0</v>
       </c>
       <c r="C163" s="7">
-        <v>858</v>
+        <v>766</v>
       </c>
       <c r="D163" s="6"/>
       <c r="E163" s="7"/>
@@ -2627,7 +2628,7 @@
         <v>0</v>
       </c>
       <c r="C164" s="7">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="D164" s="6"/>
       <c r="E164" s="7"/>
@@ -2640,7 +2641,7 @@
         <v>0</v>
       </c>
       <c r="C165" s="7">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="D165" s="6"/>
       <c r="E165" s="7"/>
@@ -2653,7 +2654,7 @@
         <v>0</v>
       </c>
       <c r="C166" s="7">
-        <v>769</v>
+        <v>892</v>
       </c>
       <c r="D166" s="6"/>
       <c r="E166" s="7"/>
@@ -2666,7 +2667,7 @@
         <v>0</v>
       </c>
       <c r="C167" s="7">
-        <v>892</v>
+        <v>119</v>
       </c>
       <c r="D167" s="6"/>
       <c r="E167" s="7"/>
@@ -2679,7 +2680,7 @@
         <v>0</v>
       </c>
       <c r="C168" s="7">
-        <v>119</v>
+        <v>920</v>
       </c>
       <c r="D168" s="6"/>
       <c r="E168" s="7"/>
@@ -2692,7 +2693,7 @@
         <v>0</v>
       </c>
       <c r="C169" s="7">
-        <v>920</v>
+        <v>956</v>
       </c>
       <c r="D169" s="6"/>
       <c r="E169" s="7"/>
@@ -2705,7 +2706,7 @@
         <v>0</v>
       </c>
       <c r="C170" s="7">
-        <v>956</v>
+        <v>1009</v>
       </c>
       <c r="D170" s="6"/>
       <c r="E170" s="7"/>
@@ -2718,7 +2719,7 @@
         <v>0</v>
       </c>
       <c r="C171" s="7">
-        <v>1009</v>
+        <v>30</v>
       </c>
       <c r="D171" s="6"/>
       <c r="E171" s="7"/>
@@ -2731,7 +2732,7 @@
         <v>0</v>
       </c>
       <c r="C172" s="7">
-        <v>30</v>
+        <v>957</v>
       </c>
       <c r="D172" s="6"/>
       <c r="E172" s="7"/>
@@ -2744,7 +2745,7 @@
         <v>0</v>
       </c>
       <c r="C173" s="7">
-        <v>957</v>
+        <v>860</v>
       </c>
       <c r="D173" s="6"/>
       <c r="E173" s="7"/>
@@ -2757,26 +2758,13 @@
         <v>0</v>
       </c>
       <c r="C174" s="7">
-        <v>860</v>
+        <v>1028</v>
       </c>
       <c r="D174" s="6"/>
       <c r="E174" s="7"/>
     </row>
-    <row r="175" spans="1:5">
-      <c r="A175" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B175" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C175" s="7">
-        <v>1028</v>
-      </c>
-      <c r="D175" s="6"/>
-      <c r="E175" s="7"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:D43">
+  <autoFilter ref="A1:D174">
     <sortState ref="A2:H43">
       <sortCondition ref="B1:B43"/>
     </sortState>

</xml_diff>

<commit_message>
Fixed Evan's cohort ischemic stroke
</commit_message>
<xml_diff>
--- a/analysis_specifications/analysis2InputSpecifications.xlsx
+++ b/analysis_specifications/analysis2InputSpecifications.xlsx
@@ -447,8 +447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="D115" sqref="D115"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="D116" sqref="D116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1997,7 +1997,7 @@
         <v>1103</v>
       </c>
       <c r="D115" s="1">
-        <v>944</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -2175,7 +2175,9 @@
       <c r="C129" s="7">
         <v>405</v>
       </c>
-      <c r="D129" s="6"/>
+      <c r="D129" s="6">
+        <v>346</v>
+      </c>
       <c r="E129" s="7"/>
     </row>
     <row r="130" spans="1:5">

</xml_diff>

<commit_message>
Update to Andreas cohorts
</commit_message>
<xml_diff>
--- a/analysis_specifications/analysis2InputSpecifications.xlsx
+++ b/analysis_specifications/analysis2InputSpecifications.xlsx
@@ -447,8 +447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="D116" sqref="D116"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D95" sqref="D63:D95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1083,7 +1083,7 @@
         <v>818</v>
       </c>
       <c r="D45" s="4">
-        <v>25</v>
+        <v>795</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1097,7 +1097,7 @@
         <v>824</v>
       </c>
       <c r="D46" s="4">
-        <v>25</v>
+        <v>796</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1111,7 +1111,7 @@
         <v>829</v>
       </c>
       <c r="D47" s="4">
-        <v>25</v>
+        <v>797</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1124,9 +1124,7 @@
       <c r="C48" s="1">
         <v>833</v>
       </c>
-      <c r="D48" s="4">
-        <v>25</v>
-      </c>
+      <c r="D48" s="4"/>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="1" t="s">
@@ -1138,9 +1136,7 @@
       <c r="C49" s="1">
         <v>838</v>
       </c>
-      <c r="D49" s="4">
-        <v>25</v>
-      </c>
+      <c r="D49" s="4"/>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="1" t="s">
@@ -1152,9 +1148,7 @@
       <c r="C50" s="1">
         <v>842</v>
       </c>
-      <c r="D50" s="4">
-        <v>25</v>
-      </c>
+      <c r="D50" s="4"/>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="1" t="s">
@@ -1180,9 +1174,7 @@
       <c r="C52" s="1">
         <v>821</v>
       </c>
-      <c r="D52" s="4">
-        <v>25</v>
-      </c>
+      <c r="D52" s="4"/>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="1" t="s">
@@ -1194,9 +1186,7 @@
       <c r="C53" s="1">
         <v>832</v>
       </c>
-      <c r="D53" s="4">
-        <v>25</v>
-      </c>
+      <c r="D53" s="4"/>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="1" t="s">
@@ -1208,9 +1198,7 @@
       <c r="C54" s="1">
         <v>836</v>
       </c>
-      <c r="D54" s="4">
-        <v>25</v>
-      </c>
+      <c r="D54" s="4"/>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="1" t="s">
@@ -1222,9 +1210,7 @@
       <c r="C55" s="1">
         <v>839</v>
       </c>
-      <c r="D55" s="4">
-        <v>25</v>
-      </c>
+      <c r="D55" s="4"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="1" t="s">
@@ -1236,9 +1222,7 @@
       <c r="C56" s="1">
         <v>848</v>
       </c>
-      <c r="D56" s="4">
-        <v>25</v>
-      </c>
+      <c r="D56" s="4"/>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="1" t="s">
@@ -1264,9 +1248,7 @@
       <c r="C58" s="1">
         <v>831</v>
       </c>
-      <c r="D58" s="4">
-        <v>25</v>
-      </c>
+      <c r="D58" s="4"/>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="1" t="s">
@@ -1278,9 +1260,7 @@
       <c r="C59" s="1">
         <v>835</v>
       </c>
-      <c r="D59" s="4">
-        <v>25</v>
-      </c>
+      <c r="D59" s="4"/>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="1" t="s">
@@ -1292,9 +1272,7 @@
       <c r="C60" s="1">
         <v>840</v>
       </c>
-      <c r="D60" s="4">
-        <v>25</v>
-      </c>
+      <c r="D60" s="4"/>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="1" t="s">
@@ -1306,9 +1284,7 @@
       <c r="C61" s="1">
         <v>843</v>
       </c>
-      <c r="D61" s="4">
-        <v>25</v>
-      </c>
+      <c r="D61" s="4"/>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="1" t="s">
@@ -1320,9 +1296,7 @@
       <c r="C62" s="1">
         <v>820</v>
       </c>
-      <c r="D62" s="4">
-        <v>25</v>
-      </c>
+      <c r="D62" s="4"/>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="1" t="s">
@@ -2767,8 +2741,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:D174">
-    <sortState ref="A2:H43">
-      <sortCondition ref="B1:B43"/>
+    <sortState ref="A45:D95">
+      <sortCondition ref="A1:A174"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Instead of Intersting Cohorts only pull cohorts in analysis 2
</commit_message>
<xml_diff>
--- a/analysis_specifications/analysis2InputSpecifications.xlsx
+++ b/analysis_specifications/analysis2InputSpecifications.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$174</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$173</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="14">
   <si>
     <t>a</t>
   </si>
@@ -445,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E174"/>
+  <dimension ref="A1:E173"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D95" sqref="D63:D95"/>
+      <selection activeCell="D94" sqref="D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1309,7 +1309,7 @@
         <v>819</v>
       </c>
       <c r="D63" s="4">
-        <v>25</v>
+        <v>811</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1323,7 +1323,7 @@
         <v>822</v>
       </c>
       <c r="D64" s="4">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1337,7 +1337,7 @@
         <v>834</v>
       </c>
       <c r="D65" s="4">
-        <v>810</v>
+        <v>854</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1351,7 +1351,7 @@
         <v>841</v>
       </c>
       <c r="D66" s="4">
-        <v>854</v>
+        <v>855</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1365,7 +1365,7 @@
         <v>830</v>
       </c>
       <c r="D67" s="4">
-        <v>855</v>
+        <v>797</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1379,7 +1379,7 @@
         <v>845</v>
       </c>
       <c r="D68" s="4">
-        <v>797</v>
+        <v>795</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -1391,7 +1391,7 @@
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="4">
-        <v>795</v>
+        <v>804</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1403,7 +1403,7 @@
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="4">
-        <v>804</v>
+        <v>805</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1415,7 +1415,7 @@
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="4">
-        <v>805</v>
+        <v>850</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1427,7 +1427,7 @@
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="4">
-        <v>850</v>
+        <v>851</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1439,7 +1439,7 @@
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="4">
-        <v>851</v>
+        <v>809</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1451,7 +1451,7 @@
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="4">
-        <v>809</v>
+        <v>852</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="4">
-        <v>852</v>
+        <v>806</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1475,7 +1475,7 @@
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="4">
-        <v>806</v>
+        <v>411</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -1487,7 +1487,7 @@
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="4">
-        <v>411</v>
+        <v>463</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -1499,7 +1499,7 @@
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="4">
-        <v>463</v>
+        <v>19</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -1511,7 +1511,7 @@
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="4">
-        <v>19</v>
+        <v>507</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1523,7 +1523,7 @@
       </c>
       <c r="C80" s="1"/>
       <c r="D80" s="4">
-        <v>507</v>
+        <v>765</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -1535,7 +1535,7 @@
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="4">
-        <v>765</v>
+        <v>766</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -1547,7 +1547,7 @@
       </c>
       <c r="C82" s="1"/>
       <c r="D82" s="4">
-        <v>766</v>
+        <v>934</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1559,7 +1559,7 @@
       </c>
       <c r="C83" s="1"/>
       <c r="D83" s="4">
-        <v>934</v>
+        <v>938</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -1571,7 +1571,7 @@
       </c>
       <c r="C84" s="1"/>
       <c r="D84" s="4">
-        <v>938</v>
+        <v>513</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -1583,7 +1583,7 @@
       </c>
       <c r="C85" s="1"/>
       <c r="D85" s="4">
-        <v>513</v>
+        <v>405</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -1595,7 +1595,7 @@
       </c>
       <c r="C86" s="1"/>
       <c r="D86" s="4">
-        <v>405</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -1607,7 +1607,7 @@
       </c>
       <c r="C87" s="1"/>
       <c r="D87" s="4">
-        <v>1081</v>
+        <v>362</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -1619,7 +1619,7 @@
       </c>
       <c r="C88" s="1"/>
       <c r="D88" s="4">
-        <v>362</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -1631,7 +1631,7 @@
       </c>
       <c r="C89" s="1"/>
       <c r="D89" s="4">
-        <v>1088</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -1643,7 +1643,7 @@
       </c>
       <c r="C90" s="1"/>
       <c r="D90" s="4">
-        <v>1090</v>
+        <v>808</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -1655,7 +1655,7 @@
       </c>
       <c r="C91" s="1"/>
       <c r="D91" s="4">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -1667,7 +1667,7 @@
       </c>
       <c r="C92" s="1"/>
       <c r="D92" s="4">
-        <v>807</v>
+        <v>410</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -1679,7 +1679,7 @@
       </c>
       <c r="C93" s="1"/>
       <c r="D93" s="4">
-        <v>410</v>
+        <v>861</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -1691,19 +1691,21 @@
       </c>
       <c r="C94" s="1"/>
       <c r="D94" s="4">
-        <v>861</v>
+        <v>803</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C95" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="C95" s="1">
+        <v>865</v>
+      </c>
       <c r="D95" s="4">
-        <v>803</v>
+        <v>965</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -1714,10 +1716,10 @@
         <v>0</v>
       </c>
       <c r="C96" s="1">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="D96" s="4">
-        <v>965</v>
+        <v>967</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -1728,10 +1730,10 @@
         <v>0</v>
       </c>
       <c r="C97" s="1">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="D97" s="4">
-        <v>967</v>
+        <v>970</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -1742,10 +1744,10 @@
         <v>0</v>
       </c>
       <c r="C98" s="1">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="D98" s="4">
-        <v>970</v>
+        <v>938</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -1756,10 +1758,10 @@
         <v>0</v>
       </c>
       <c r="C99" s="1">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="D99" s="4">
-        <v>938</v>
+        <v>934</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -1770,10 +1772,10 @@
         <v>0</v>
       </c>
       <c r="C100" s="1">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="D100" s="4">
-        <v>934</v>
+        <v>513</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -1784,10 +1786,10 @@
         <v>0</v>
       </c>
       <c r="C101" s="1">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="D101" s="4">
-        <v>513</v>
+        <v>405</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -1798,10 +1800,10 @@
         <v>0</v>
       </c>
       <c r="C102" s="1">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="D102" s="4">
-        <v>405</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -1812,10 +1814,10 @@
         <v>0</v>
       </c>
       <c r="C103" s="1">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="D103" s="4">
-        <v>1081</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -1826,10 +1828,10 @@
         <v>0</v>
       </c>
       <c r="C104" s="1">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="D104" s="4">
-        <v>1088</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -1840,10 +1842,10 @@
         <v>0</v>
       </c>
       <c r="C105" s="1">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="D105" s="4">
-        <v>1090</v>
+        <v>19</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -1854,10 +1856,10 @@
         <v>0</v>
       </c>
       <c r="C106" s="1">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="D106" s="4">
-        <v>19</v>
+        <v>507</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -1867,11 +1869,9 @@
       <c r="B107" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C107" s="1">
-        <v>876</v>
-      </c>
+      <c r="C107" s="1"/>
       <c r="D107" s="4">
-        <v>507</v>
+        <v>410</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -1883,7 +1883,7 @@
       </c>
       <c r="C108" s="1"/>
       <c r="D108" s="4">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -1895,7 +1895,7 @@
       </c>
       <c r="C109" s="1"/>
       <c r="D109" s="4">
-        <v>411</v>
+        <v>463</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -1907,7 +1907,7 @@
       </c>
       <c r="C110" s="1"/>
       <c r="D110" s="4">
-        <v>463</v>
+        <v>362</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -1919,7 +1919,7 @@
       </c>
       <c r="C111" s="1"/>
       <c r="D111" s="4">
-        <v>362</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -1931,7 +1931,7 @@
       </c>
       <c r="C112" s="1"/>
       <c r="D112" s="4">
-        <v>1104</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -1939,11 +1939,13 @@
         <v>8</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C113" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="C113" s="1">
+        <v>1106</v>
+      </c>
       <c r="D113" s="4">
-        <v>1105</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -1954,10 +1956,10 @@
         <v>1</v>
       </c>
       <c r="C114" s="1">
-        <v>1106</v>
-      </c>
-      <c r="D114" s="4">
-        <v>1081</v>
+        <v>1103</v>
+      </c>
+      <c r="D114" s="1">
+        <v>1089</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -1968,11 +1970,9 @@
         <v>1</v>
       </c>
       <c r="C115" s="1">
-        <v>1103</v>
-      </c>
-      <c r="D115" s="1">
-        <v>1089</v>
-      </c>
+        <v>1102</v>
+      </c>
+      <c r="D115" s="1"/>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="1" t="s">
@@ -1982,7 +1982,7 @@
         <v>1</v>
       </c>
       <c r="C116" s="1">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="D116" s="1"/>
     </row>
@@ -1994,7 +1994,7 @@
         <v>1</v>
       </c>
       <c r="C117" s="1">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="D117" s="1"/>
     </row>
@@ -2006,7 +2006,7 @@
         <v>1</v>
       </c>
       <c r="C118" s="1">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="D118" s="1"/>
     </row>
@@ -2018,7 +2018,7 @@
         <v>1</v>
       </c>
       <c r="C119" s="1">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="D119" s="1"/>
     </row>
@@ -2030,7 +2030,7 @@
         <v>1</v>
       </c>
       <c r="C120" s="1">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="D120" s="1"/>
     </row>
@@ -2042,7 +2042,7 @@
         <v>1</v>
       </c>
       <c r="C121" s="1">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="D121" s="1"/>
     </row>
@@ -2054,7 +2054,7 @@
         <v>1</v>
       </c>
       <c r="C122" s="1">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="D122" s="1"/>
     </row>
@@ -2066,7 +2066,7 @@
         <v>1</v>
       </c>
       <c r="C123" s="1">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="D123" s="1"/>
     </row>
@@ -2078,34 +2078,37 @@
         <v>1</v>
       </c>
       <c r="C124" s="1">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="D124" s="1"/>
     </row>
     <row r="125" spans="1:5">
-      <c r="A125" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B125" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C125" s="1">
-        <v>1093</v>
-      </c>
-      <c r="D125" s="1"/>
+      <c r="A125" t="s">
+        <v>13</v>
+      </c>
+      <c r="B125" t="s">
+        <v>0</v>
+      </c>
+      <c r="C125" s="7">
+        <v>723</v>
+      </c>
+      <c r="D125" s="7">
+        <v>24</v>
+      </c>
+      <c r="E125" s="7"/>
     </row>
     <row r="126" spans="1:5">
-      <c r="A126" t="s">
-        <v>13</v>
-      </c>
-      <c r="B126" t="s">
+      <c r="A126" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B126" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C126" s="7">
-        <v>723</v>
+        <v>716</v>
       </c>
       <c r="D126" s="7">
-        <v>24</v>
+        <v>707</v>
       </c>
       <c r="E126" s="7"/>
     </row>
@@ -2117,10 +2120,10 @@
         <v>0</v>
       </c>
       <c r="C127" s="7">
-        <v>716</v>
+        <v>1081</v>
       </c>
       <c r="D127" s="7">
-        <v>707</v>
+        <v>347</v>
       </c>
       <c r="E127" s="7"/>
     </row>
@@ -2132,10 +2135,10 @@
         <v>0</v>
       </c>
       <c r="C128" s="7">
-        <v>1081</v>
-      </c>
-      <c r="D128" s="7">
-        <v>347</v>
+        <v>405</v>
+      </c>
+      <c r="D128" s="6">
+        <v>346</v>
       </c>
       <c r="E128" s="7"/>
     </row>
@@ -2147,11 +2150,9 @@
         <v>0</v>
       </c>
       <c r="C129" s="7">
-        <v>405</v>
-      </c>
-      <c r="D129" s="6">
-        <v>346</v>
-      </c>
+        <v>251</v>
+      </c>
+      <c r="D129" s="6"/>
       <c r="E129" s="7"/>
     </row>
     <row r="130" spans="1:5">
@@ -2162,7 +2163,7 @@
         <v>0</v>
       </c>
       <c r="C130" s="7">
-        <v>251</v>
+        <v>735</v>
       </c>
       <c r="D130" s="6"/>
       <c r="E130" s="7"/>
@@ -2175,7 +2176,7 @@
         <v>0</v>
       </c>
       <c r="C131" s="7">
-        <v>735</v>
+        <v>729</v>
       </c>
       <c r="D131" s="6"/>
       <c r="E131" s="7"/>
@@ -2188,7 +2189,7 @@
         <v>0</v>
       </c>
       <c r="C132" s="7">
-        <v>729</v>
+        <v>862</v>
       </c>
       <c r="D132" s="6"/>
       <c r="E132" s="7"/>
@@ -2201,7 +2202,7 @@
         <v>0</v>
       </c>
       <c r="C133" s="7">
-        <v>862</v>
+        <v>1013</v>
       </c>
       <c r="D133" s="6"/>
       <c r="E133" s="7"/>
@@ -2214,7 +2215,7 @@
         <v>0</v>
       </c>
       <c r="C134" s="7">
-        <v>1013</v>
+        <v>334</v>
       </c>
       <c r="D134" s="6"/>
       <c r="E134" s="7"/>
@@ -2227,7 +2228,7 @@
         <v>0</v>
       </c>
       <c r="C135" s="7">
-        <v>334</v>
+        <v>989</v>
       </c>
       <c r="D135" s="6"/>
       <c r="E135" s="7"/>
@@ -2240,7 +2241,7 @@
         <v>0</v>
       </c>
       <c r="C136" s="7">
-        <v>989</v>
+        <v>923</v>
       </c>
       <c r="D136" s="6"/>
       <c r="E136" s="7"/>
@@ -2253,7 +2254,7 @@
         <v>0</v>
       </c>
       <c r="C137" s="7">
-        <v>923</v>
+        <v>1027</v>
       </c>
       <c r="D137" s="6"/>
       <c r="E137" s="7"/>
@@ -2266,7 +2267,7 @@
         <v>0</v>
       </c>
       <c r="C138" s="7">
-        <v>1027</v>
+        <v>710</v>
       </c>
       <c r="D138" s="6"/>
       <c r="E138" s="7"/>
@@ -2279,7 +2280,7 @@
         <v>0</v>
       </c>
       <c r="C139" s="7">
-        <v>710</v>
+        <v>1031</v>
       </c>
       <c r="D139" s="6"/>
       <c r="E139" s="7"/>
@@ -2292,7 +2293,7 @@
         <v>0</v>
       </c>
       <c r="C140" s="7">
-        <v>1031</v>
+        <v>859</v>
       </c>
       <c r="D140" s="6"/>
       <c r="E140" s="7"/>
@@ -2305,7 +2306,7 @@
         <v>0</v>
       </c>
       <c r="C141" s="7">
-        <v>859</v>
+        <v>1007</v>
       </c>
       <c r="D141" s="6"/>
       <c r="E141" s="7"/>
@@ -2318,7 +2319,7 @@
         <v>0</v>
       </c>
       <c r="C142" s="7">
-        <v>1007</v>
+        <v>770</v>
       </c>
       <c r="D142" s="6"/>
       <c r="E142" s="7"/>
@@ -2331,7 +2332,7 @@
         <v>0</v>
       </c>
       <c r="C143" s="7">
-        <v>770</v>
+        <v>667</v>
       </c>
       <c r="D143" s="6"/>
       <c r="E143" s="7"/>
@@ -2344,7 +2345,7 @@
         <v>0</v>
       </c>
       <c r="C144" s="7">
-        <v>667</v>
+        <v>934</v>
       </c>
       <c r="D144" s="6"/>
       <c r="E144" s="7"/>
@@ -2357,7 +2358,7 @@
         <v>0</v>
       </c>
       <c r="C145" s="7">
-        <v>934</v>
+        <v>1087</v>
       </c>
       <c r="D145" s="6"/>
       <c r="E145" s="7"/>
@@ -2370,7 +2371,7 @@
         <v>0</v>
       </c>
       <c r="C146" s="7">
-        <v>1087</v>
+        <v>715</v>
       </c>
       <c r="D146" s="6"/>
       <c r="E146" s="7"/>
@@ -2383,7 +2384,7 @@
         <v>0</v>
       </c>
       <c r="C147" s="7">
-        <v>715</v>
+        <v>1083</v>
       </c>
       <c r="D147" s="6"/>
       <c r="E147" s="7"/>
@@ -2396,7 +2397,7 @@
         <v>0</v>
       </c>
       <c r="C148" s="7">
-        <v>1083</v>
+        <v>745</v>
       </c>
       <c r="D148" s="6"/>
       <c r="E148" s="7"/>
@@ -2409,7 +2410,7 @@
         <v>0</v>
       </c>
       <c r="C149" s="7">
-        <v>745</v>
+        <v>765</v>
       </c>
       <c r="D149" s="6"/>
       <c r="E149" s="7"/>
@@ -2422,7 +2423,7 @@
         <v>0</v>
       </c>
       <c r="C150" s="7">
-        <v>765</v>
+        <v>1020</v>
       </c>
       <c r="D150" s="6"/>
       <c r="E150" s="7"/>
@@ -2435,7 +2436,7 @@
         <v>0</v>
       </c>
       <c r="C151" s="7">
-        <v>1020</v>
+        <v>1029</v>
       </c>
       <c r="D151" s="6"/>
       <c r="E151" s="7"/>
@@ -2448,7 +2449,7 @@
         <v>0</v>
       </c>
       <c r="C152" s="7">
-        <v>1029</v>
+        <v>1011</v>
       </c>
       <c r="D152" s="6"/>
       <c r="E152" s="7"/>
@@ -2461,7 +2462,7 @@
         <v>0</v>
       </c>
       <c r="C153" s="7">
-        <v>1011</v>
+        <v>1026</v>
       </c>
       <c r="D153" s="6"/>
       <c r="E153" s="7"/>
@@ -2474,7 +2475,7 @@
         <v>0</v>
       </c>
       <c r="C154" s="7">
-        <v>1026</v>
+        <v>919</v>
       </c>
       <c r="D154" s="6"/>
       <c r="E154" s="7"/>
@@ -2487,7 +2488,7 @@
         <v>0</v>
       </c>
       <c r="C155" s="7">
-        <v>919</v>
+        <v>749</v>
       </c>
       <c r="D155" s="6"/>
       <c r="E155" s="7"/>
@@ -2500,7 +2501,7 @@
         <v>0</v>
       </c>
       <c r="C156" s="7">
-        <v>749</v>
+        <v>1030</v>
       </c>
       <c r="D156" s="6"/>
       <c r="E156" s="7"/>
@@ -2513,7 +2514,7 @@
         <v>0</v>
       </c>
       <c r="C157" s="7">
-        <v>1030</v>
+        <v>748</v>
       </c>
       <c r="D157" s="6"/>
       <c r="E157" s="7"/>
@@ -2526,7 +2527,7 @@
         <v>0</v>
       </c>
       <c r="C158" s="7">
-        <v>748</v>
+        <v>744</v>
       </c>
       <c r="D158" s="6"/>
       <c r="E158" s="7"/>
@@ -2539,7 +2540,7 @@
         <v>0</v>
       </c>
       <c r="C159" s="7">
-        <v>744</v>
+        <v>1003</v>
       </c>
       <c r="D159" s="6"/>
       <c r="E159" s="7"/>
@@ -2552,7 +2553,7 @@
         <v>0</v>
       </c>
       <c r="C160" s="7">
-        <v>1003</v>
+        <v>43</v>
       </c>
       <c r="D160" s="6"/>
       <c r="E160" s="7"/>
@@ -2565,7 +2566,7 @@
         <v>0</v>
       </c>
       <c r="C161" s="7">
-        <v>43</v>
+        <v>858</v>
       </c>
       <c r="D161" s="6"/>
       <c r="E161" s="7"/>
@@ -2578,7 +2579,7 @@
         <v>0</v>
       </c>
       <c r="C162" s="7">
-        <v>858</v>
+        <v>766</v>
       </c>
       <c r="D162" s="6"/>
       <c r="E162" s="7"/>
@@ -2591,7 +2592,7 @@
         <v>0</v>
       </c>
       <c r="C163" s="7">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="D163" s="6"/>
       <c r="E163" s="7"/>
@@ -2604,7 +2605,7 @@
         <v>0</v>
       </c>
       <c r="C164" s="7">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="D164" s="6"/>
       <c r="E164" s="7"/>
@@ -2617,7 +2618,7 @@
         <v>0</v>
       </c>
       <c r="C165" s="7">
-        <v>769</v>
+        <v>892</v>
       </c>
       <c r="D165" s="6"/>
       <c r="E165" s="7"/>
@@ -2630,7 +2631,7 @@
         <v>0</v>
       </c>
       <c r="C166" s="7">
-        <v>892</v>
+        <v>119</v>
       </c>
       <c r="D166" s="6"/>
       <c r="E166" s="7"/>
@@ -2643,7 +2644,7 @@
         <v>0</v>
       </c>
       <c r="C167" s="7">
-        <v>119</v>
+        <v>920</v>
       </c>
       <c r="D167" s="6"/>
       <c r="E167" s="7"/>
@@ -2656,7 +2657,7 @@
         <v>0</v>
       </c>
       <c r="C168" s="7">
-        <v>920</v>
+        <v>956</v>
       </c>
       <c r="D168" s="6"/>
       <c r="E168" s="7"/>
@@ -2669,7 +2670,7 @@
         <v>0</v>
       </c>
       <c r="C169" s="7">
-        <v>956</v>
+        <v>1009</v>
       </c>
       <c r="D169" s="6"/>
       <c r="E169" s="7"/>
@@ -2682,7 +2683,7 @@
         <v>0</v>
       </c>
       <c r="C170" s="7">
-        <v>1009</v>
+        <v>30</v>
       </c>
       <c r="D170" s="6"/>
       <c r="E170" s="7"/>
@@ -2695,7 +2696,7 @@
         <v>0</v>
       </c>
       <c r="C171" s="7">
-        <v>30</v>
+        <v>957</v>
       </c>
       <c r="D171" s="6"/>
       <c r="E171" s="7"/>
@@ -2708,7 +2709,7 @@
         <v>0</v>
       </c>
       <c r="C172" s="7">
-        <v>957</v>
+        <v>860</v>
       </c>
       <c r="D172" s="6"/>
       <c r="E172" s="7"/>
@@ -2721,26 +2722,13 @@
         <v>0</v>
       </c>
       <c r="C173" s="7">
-        <v>860</v>
+        <v>1028</v>
       </c>
       <c r="D173" s="6"/>
       <c r="E173" s="7"/>
     </row>
-    <row r="174" spans="1:5">
-      <c r="A174" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B174" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C174" s="7">
-        <v>1028</v>
-      </c>
-      <c r="D174" s="6"/>
-      <c r="E174" s="7"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:D174">
+  <autoFilter ref="A1:D173">
     <sortState ref="A45:D95">
       <sortCondition ref="A1:A174"/>
     </sortState>

</xml_diff>

<commit_message>
remove 803 from andrea
</commit_message>
<xml_diff>
--- a/analysis_specifications/analysis2InputSpecifications.xlsx
+++ b/analysis_specifications/analysis2InputSpecifications.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$173</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$172</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="14">
   <si>
     <t>a</t>
   </si>
@@ -445,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E173"/>
+  <dimension ref="A1:E172"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D94" sqref="D94"/>
+      <selection activeCell="A94" sqref="A94:XFD94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1684,14 +1684,16 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C94" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="C94" s="1">
+        <v>865</v>
+      </c>
       <c r="D94" s="4">
-        <v>803</v>
+        <v>965</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -1702,10 +1704,10 @@
         <v>0</v>
       </c>
       <c r="C95" s="1">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="D95" s="4">
-        <v>965</v>
+        <v>967</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -1716,10 +1718,10 @@
         <v>0</v>
       </c>
       <c r="C96" s="1">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="D96" s="4">
-        <v>967</v>
+        <v>970</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -1730,10 +1732,10 @@
         <v>0</v>
       </c>
       <c r="C97" s="1">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="D97" s="4">
-        <v>970</v>
+        <v>938</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -1744,10 +1746,10 @@
         <v>0</v>
       </c>
       <c r="C98" s="1">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="D98" s="4">
-        <v>938</v>
+        <v>934</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -1758,10 +1760,10 @@
         <v>0</v>
       </c>
       <c r="C99" s="1">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="D99" s="4">
-        <v>934</v>
+        <v>513</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -1772,10 +1774,10 @@
         <v>0</v>
       </c>
       <c r="C100" s="1">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="D100" s="4">
-        <v>513</v>
+        <v>405</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -1786,10 +1788,10 @@
         <v>0</v>
       </c>
       <c r="C101" s="1">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="D101" s="4">
-        <v>405</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -1800,10 +1802,10 @@
         <v>0</v>
       </c>
       <c r="C102" s="1">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="D102" s="4">
-        <v>1081</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -1814,10 +1816,10 @@
         <v>0</v>
       </c>
       <c r="C103" s="1">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="D103" s="4">
-        <v>1088</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -1828,10 +1830,10 @@
         <v>0</v>
       </c>
       <c r="C104" s="1">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="D104" s="4">
-        <v>1090</v>
+        <v>19</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -1842,10 +1844,10 @@
         <v>0</v>
       </c>
       <c r="C105" s="1">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="D105" s="4">
-        <v>19</v>
+        <v>507</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -1855,11 +1857,9 @@
       <c r="B106" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C106" s="1">
-        <v>876</v>
-      </c>
+      <c r="C106" s="1"/>
       <c r="D106" s="4">
-        <v>507</v>
+        <v>410</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -1871,7 +1871,7 @@
       </c>
       <c r="C107" s="1"/>
       <c r="D107" s="4">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -1883,7 +1883,7 @@
       </c>
       <c r="C108" s="1"/>
       <c r="D108" s="4">
-        <v>411</v>
+        <v>463</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -1895,7 +1895,7 @@
       </c>
       <c r="C109" s="1"/>
       <c r="D109" s="4">
-        <v>463</v>
+        <v>362</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -1907,7 +1907,7 @@
       </c>
       <c r="C110" s="1"/>
       <c r="D110" s="4">
-        <v>362</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -1919,7 +1919,7 @@
       </c>
       <c r="C111" s="1"/>
       <c r="D111" s="4">
-        <v>1104</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -1927,11 +1927,13 @@
         <v>8</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C112" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="C112" s="1">
+        <v>1106</v>
+      </c>
       <c r="D112" s="4">
-        <v>1105</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -1942,10 +1944,10 @@
         <v>1</v>
       </c>
       <c r="C113" s="1">
-        <v>1106</v>
-      </c>
-      <c r="D113" s="4">
-        <v>1081</v>
+        <v>1103</v>
+      </c>
+      <c r="D113" s="1">
+        <v>1089</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -1956,11 +1958,9 @@
         <v>1</v>
       </c>
       <c r="C114" s="1">
-        <v>1103</v>
-      </c>
-      <c r="D114" s="1">
-        <v>1089</v>
-      </c>
+        <v>1102</v>
+      </c>
+      <c r="D114" s="1"/>
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="1" t="s">
@@ -1970,7 +1970,7 @@
         <v>1</v>
       </c>
       <c r="C115" s="1">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="D115" s="1"/>
     </row>
@@ -1982,7 +1982,7 @@
         <v>1</v>
       </c>
       <c r="C116" s="1">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="D116" s="1"/>
     </row>
@@ -1994,7 +1994,7 @@
         <v>1</v>
       </c>
       <c r="C117" s="1">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="D117" s="1"/>
     </row>
@@ -2006,7 +2006,7 @@
         <v>1</v>
       </c>
       <c r="C118" s="1">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="D118" s="1"/>
     </row>
@@ -2018,7 +2018,7 @@
         <v>1</v>
       </c>
       <c r="C119" s="1">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="D119" s="1"/>
     </row>
@@ -2030,7 +2030,7 @@
         <v>1</v>
       </c>
       <c r="C120" s="1">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="D120" s="1"/>
     </row>
@@ -2042,7 +2042,7 @@
         <v>1</v>
       </c>
       <c r="C121" s="1">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="D121" s="1"/>
     </row>
@@ -2054,7 +2054,7 @@
         <v>1</v>
       </c>
       <c r="C122" s="1">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="D122" s="1"/>
     </row>
@@ -2066,34 +2066,37 @@
         <v>1</v>
       </c>
       <c r="C123" s="1">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="D123" s="1"/>
     </row>
     <row r="124" spans="1:5">
-      <c r="A124" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B124" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C124" s="1">
-        <v>1093</v>
-      </c>
-      <c r="D124" s="1"/>
+      <c r="A124" t="s">
+        <v>13</v>
+      </c>
+      <c r="B124" t="s">
+        <v>0</v>
+      </c>
+      <c r="C124" s="7">
+        <v>723</v>
+      </c>
+      <c r="D124" s="7">
+        <v>24</v>
+      </c>
+      <c r="E124" s="7"/>
     </row>
     <row r="125" spans="1:5">
-      <c r="A125" t="s">
-        <v>13</v>
-      </c>
-      <c r="B125" t="s">
+      <c r="A125" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B125" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C125" s="7">
-        <v>723</v>
+        <v>716</v>
       </c>
       <c r="D125" s="7">
-        <v>24</v>
+        <v>707</v>
       </c>
       <c r="E125" s="7"/>
     </row>
@@ -2105,10 +2108,10 @@
         <v>0</v>
       </c>
       <c r="C126" s="7">
-        <v>716</v>
+        <v>1081</v>
       </c>
       <c r="D126" s="7">
-        <v>707</v>
+        <v>347</v>
       </c>
       <c r="E126" s="7"/>
     </row>
@@ -2120,10 +2123,10 @@
         <v>0</v>
       </c>
       <c r="C127" s="7">
-        <v>1081</v>
-      </c>
-      <c r="D127" s="7">
-        <v>347</v>
+        <v>405</v>
+      </c>
+      <c r="D127" s="6">
+        <v>346</v>
       </c>
       <c r="E127" s="7"/>
     </row>
@@ -2135,11 +2138,9 @@
         <v>0</v>
       </c>
       <c r="C128" s="7">
-        <v>405</v>
-      </c>
-      <c r="D128" s="6">
-        <v>346</v>
-      </c>
+        <v>251</v>
+      </c>
+      <c r="D128" s="6"/>
       <c r="E128" s="7"/>
     </row>
     <row r="129" spans="1:5">
@@ -2150,7 +2151,7 @@
         <v>0</v>
       </c>
       <c r="C129" s="7">
-        <v>251</v>
+        <v>735</v>
       </c>
       <c r="D129" s="6"/>
       <c r="E129" s="7"/>
@@ -2163,7 +2164,7 @@
         <v>0</v>
       </c>
       <c r="C130" s="7">
-        <v>735</v>
+        <v>729</v>
       </c>
       <c r="D130" s="6"/>
       <c r="E130" s="7"/>
@@ -2176,7 +2177,7 @@
         <v>0</v>
       </c>
       <c r="C131" s="7">
-        <v>729</v>
+        <v>862</v>
       </c>
       <c r="D131" s="6"/>
       <c r="E131" s="7"/>
@@ -2189,7 +2190,7 @@
         <v>0</v>
       </c>
       <c r="C132" s="7">
-        <v>862</v>
+        <v>1013</v>
       </c>
       <c r="D132" s="6"/>
       <c r="E132" s="7"/>
@@ -2202,7 +2203,7 @@
         <v>0</v>
       </c>
       <c r="C133" s="7">
-        <v>1013</v>
+        <v>334</v>
       </c>
       <c r="D133" s="6"/>
       <c r="E133" s="7"/>
@@ -2215,7 +2216,7 @@
         <v>0</v>
       </c>
       <c r="C134" s="7">
-        <v>334</v>
+        <v>989</v>
       </c>
       <c r="D134" s="6"/>
       <c r="E134" s="7"/>
@@ -2228,7 +2229,7 @@
         <v>0</v>
       </c>
       <c r="C135" s="7">
-        <v>989</v>
+        <v>923</v>
       </c>
       <c r="D135" s="6"/>
       <c r="E135" s="7"/>
@@ -2241,7 +2242,7 @@
         <v>0</v>
       </c>
       <c r="C136" s="7">
-        <v>923</v>
+        <v>1027</v>
       </c>
       <c r="D136" s="6"/>
       <c r="E136" s="7"/>
@@ -2254,7 +2255,7 @@
         <v>0</v>
       </c>
       <c r="C137" s="7">
-        <v>1027</v>
+        <v>710</v>
       </c>
       <c r="D137" s="6"/>
       <c r="E137" s="7"/>
@@ -2267,7 +2268,7 @@
         <v>0</v>
       </c>
       <c r="C138" s="7">
-        <v>710</v>
+        <v>1031</v>
       </c>
       <c r="D138" s="6"/>
       <c r="E138" s="7"/>
@@ -2280,7 +2281,7 @@
         <v>0</v>
       </c>
       <c r="C139" s="7">
-        <v>1031</v>
+        <v>859</v>
       </c>
       <c r="D139" s="6"/>
       <c r="E139" s="7"/>
@@ -2293,7 +2294,7 @@
         <v>0</v>
       </c>
       <c r="C140" s="7">
-        <v>859</v>
+        <v>1007</v>
       </c>
       <c r="D140" s="6"/>
       <c r="E140" s="7"/>
@@ -2306,7 +2307,7 @@
         <v>0</v>
       </c>
       <c r="C141" s="7">
-        <v>1007</v>
+        <v>770</v>
       </c>
       <c r="D141" s="6"/>
       <c r="E141" s="7"/>
@@ -2319,7 +2320,7 @@
         <v>0</v>
       </c>
       <c r="C142" s="7">
-        <v>770</v>
+        <v>667</v>
       </c>
       <c r="D142" s="6"/>
       <c r="E142" s="7"/>
@@ -2332,7 +2333,7 @@
         <v>0</v>
       </c>
       <c r="C143" s="7">
-        <v>667</v>
+        <v>934</v>
       </c>
       <c r="D143" s="6"/>
       <c r="E143" s="7"/>
@@ -2345,7 +2346,7 @@
         <v>0</v>
       </c>
       <c r="C144" s="7">
-        <v>934</v>
+        <v>1087</v>
       </c>
       <c r="D144" s="6"/>
       <c r="E144" s="7"/>
@@ -2358,7 +2359,7 @@
         <v>0</v>
       </c>
       <c r="C145" s="7">
-        <v>1087</v>
+        <v>715</v>
       </c>
       <c r="D145" s="6"/>
       <c r="E145" s="7"/>
@@ -2371,7 +2372,7 @@
         <v>0</v>
       </c>
       <c r="C146" s="7">
-        <v>715</v>
+        <v>1083</v>
       </c>
       <c r="D146" s="6"/>
       <c r="E146" s="7"/>
@@ -2384,7 +2385,7 @@
         <v>0</v>
       </c>
       <c r="C147" s="7">
-        <v>1083</v>
+        <v>745</v>
       </c>
       <c r="D147" s="6"/>
       <c r="E147" s="7"/>
@@ -2397,7 +2398,7 @@
         <v>0</v>
       </c>
       <c r="C148" s="7">
-        <v>745</v>
+        <v>765</v>
       </c>
       <c r="D148" s="6"/>
       <c r="E148" s="7"/>
@@ -2410,7 +2411,7 @@
         <v>0</v>
       </c>
       <c r="C149" s="7">
-        <v>765</v>
+        <v>1020</v>
       </c>
       <c r="D149" s="6"/>
       <c r="E149" s="7"/>
@@ -2423,7 +2424,7 @@
         <v>0</v>
       </c>
       <c r="C150" s="7">
-        <v>1020</v>
+        <v>1029</v>
       </c>
       <c r="D150" s="6"/>
       <c r="E150" s="7"/>
@@ -2436,7 +2437,7 @@
         <v>0</v>
       </c>
       <c r="C151" s="7">
-        <v>1029</v>
+        <v>1011</v>
       </c>
       <c r="D151" s="6"/>
       <c r="E151" s="7"/>
@@ -2449,7 +2450,7 @@
         <v>0</v>
       </c>
       <c r="C152" s="7">
-        <v>1011</v>
+        <v>1026</v>
       </c>
       <c r="D152" s="6"/>
       <c r="E152" s="7"/>
@@ -2462,7 +2463,7 @@
         <v>0</v>
       </c>
       <c r="C153" s="7">
-        <v>1026</v>
+        <v>919</v>
       </c>
       <c r="D153" s="6"/>
       <c r="E153" s="7"/>
@@ -2475,7 +2476,7 @@
         <v>0</v>
       </c>
       <c r="C154" s="7">
-        <v>919</v>
+        <v>749</v>
       </c>
       <c r="D154" s="6"/>
       <c r="E154" s="7"/>
@@ -2488,7 +2489,7 @@
         <v>0</v>
       </c>
       <c r="C155" s="7">
-        <v>749</v>
+        <v>1030</v>
       </c>
       <c r="D155" s="6"/>
       <c r="E155" s="7"/>
@@ -2501,7 +2502,7 @@
         <v>0</v>
       </c>
       <c r="C156" s="7">
-        <v>1030</v>
+        <v>748</v>
       </c>
       <c r="D156" s="6"/>
       <c r="E156" s="7"/>
@@ -2514,7 +2515,7 @@
         <v>0</v>
       </c>
       <c r="C157" s="7">
-        <v>748</v>
+        <v>744</v>
       </c>
       <c r="D157" s="6"/>
       <c r="E157" s="7"/>
@@ -2527,7 +2528,7 @@
         <v>0</v>
       </c>
       <c r="C158" s="7">
-        <v>744</v>
+        <v>1003</v>
       </c>
       <c r="D158" s="6"/>
       <c r="E158" s="7"/>
@@ -2540,7 +2541,7 @@
         <v>0</v>
       </c>
       <c r="C159" s="7">
-        <v>1003</v>
+        <v>43</v>
       </c>
       <c r="D159" s="6"/>
       <c r="E159" s="7"/>
@@ -2553,7 +2554,7 @@
         <v>0</v>
       </c>
       <c r="C160" s="7">
-        <v>43</v>
+        <v>858</v>
       </c>
       <c r="D160" s="6"/>
       <c r="E160" s="7"/>
@@ -2566,7 +2567,7 @@
         <v>0</v>
       </c>
       <c r="C161" s="7">
-        <v>858</v>
+        <v>766</v>
       </c>
       <c r="D161" s="6"/>
       <c r="E161" s="7"/>
@@ -2579,7 +2580,7 @@
         <v>0</v>
       </c>
       <c r="C162" s="7">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="D162" s="6"/>
       <c r="E162" s="7"/>
@@ -2592,7 +2593,7 @@
         <v>0</v>
       </c>
       <c r="C163" s="7">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="D163" s="6"/>
       <c r="E163" s="7"/>
@@ -2605,7 +2606,7 @@
         <v>0</v>
       </c>
       <c r="C164" s="7">
-        <v>769</v>
+        <v>892</v>
       </c>
       <c r="D164" s="6"/>
       <c r="E164" s="7"/>
@@ -2618,7 +2619,7 @@
         <v>0</v>
       </c>
       <c r="C165" s="7">
-        <v>892</v>
+        <v>119</v>
       </c>
       <c r="D165" s="6"/>
       <c r="E165" s="7"/>
@@ -2631,7 +2632,7 @@
         <v>0</v>
       </c>
       <c r="C166" s="7">
-        <v>119</v>
+        <v>920</v>
       </c>
       <c r="D166" s="6"/>
       <c r="E166" s="7"/>
@@ -2644,7 +2645,7 @@
         <v>0</v>
       </c>
       <c r="C167" s="7">
-        <v>920</v>
+        <v>956</v>
       </c>
       <c r="D167" s="6"/>
       <c r="E167" s="7"/>
@@ -2657,7 +2658,7 @@
         <v>0</v>
       </c>
       <c r="C168" s="7">
-        <v>956</v>
+        <v>1009</v>
       </c>
       <c r="D168" s="6"/>
       <c r="E168" s="7"/>
@@ -2670,7 +2671,7 @@
         <v>0</v>
       </c>
       <c r="C169" s="7">
-        <v>1009</v>
+        <v>30</v>
       </c>
       <c r="D169" s="6"/>
       <c r="E169" s="7"/>
@@ -2683,7 +2684,7 @@
         <v>0</v>
       </c>
       <c r="C170" s="7">
-        <v>30</v>
+        <v>957</v>
       </c>
       <c r="D170" s="6"/>
       <c r="E170" s="7"/>
@@ -2696,7 +2697,7 @@
         <v>0</v>
       </c>
       <c r="C171" s="7">
-        <v>957</v>
+        <v>860</v>
       </c>
       <c r="D171" s="6"/>
       <c r="E171" s="7"/>
@@ -2709,26 +2710,13 @@
         <v>0</v>
       </c>
       <c r="C172" s="7">
-        <v>860</v>
+        <v>1028</v>
       </c>
       <c r="D172" s="6"/>
       <c r="E172" s="7"/>
     </row>
-    <row r="173" spans="1:5">
-      <c r="A173" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B173" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C173" s="7">
-        <v>1028</v>
-      </c>
-      <c r="D173" s="6"/>
-      <c r="E173" s="7"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:D173">
+  <autoFilter ref="A1:D172">
     <sortState ref="A45:D95">
       <sortCondition ref="A1:A174"/>
     </sortState>

</xml_diff>

<commit_message>
Update joels missing mace
</commit_message>
<xml_diff>
--- a/analysis_specifications/analysis2InputSpecifications.xlsx
+++ b/analysis_specifications/analysis2InputSpecifications.xlsx
@@ -13,9 +13,10 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$172</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$154</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="14">
   <si>
     <t>a</t>
   </si>
@@ -75,7 +76,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,6 +102,20 @@
       <name val="Source Sans Pro"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -122,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -131,6 +146,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E172"/>
+  <dimension ref="A1:E154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94:XFD94"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -673,11 +690,11 @@
       <c r="B16" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="1">
-        <v>750</v>
-      </c>
-      <c r="D16" s="1">
-        <v>751</v>
+      <c r="C16" s="8">
+        <v>746</v>
+      </c>
+      <c r="D16" s="8">
+        <v>746</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -687,10 +704,10 @@
       <c r="B17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="1">
-        <v>750</v>
-      </c>
-      <c r="D17" s="1">
+      <c r="C17" s="8">
+        <v>747</v>
+      </c>
+      <c r="D17" s="8">
         <v>747</v>
       </c>
     </row>
@@ -701,11 +718,11 @@
       <c r="B18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="8">
         <v>750</v>
       </c>
-      <c r="D18" s="1">
-        <v>746</v>
+      <c r="D18" s="8">
+        <v>750</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -715,11 +732,11 @@
       <c r="B19" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="8">
         <v>751</v>
       </c>
-      <c r="D19" s="1">
-        <v>750</v>
+      <c r="D19" s="8">
+        <v>751</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -727,13 +744,13 @@
         <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="1">
-        <v>751</v>
+        <v>4</v>
+      </c>
+      <c r="C20" s="7">
+        <v>748</v>
       </c>
       <c r="D20" s="1">
-        <v>747</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -741,13 +758,13 @@
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="1">
-        <v>751</v>
-      </c>
-      <c r="D21" s="1">
-        <v>746</v>
+        <v>4</v>
+      </c>
+      <c r="C21" s="7">
+        <v>749</v>
+      </c>
+      <c r="D21" s="7">
+        <v>1074</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -755,13 +772,13 @@
         <v>5</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="1">
-        <v>747</v>
-      </c>
-      <c r="D22" s="1">
-        <v>750</v>
+        <v>4</v>
+      </c>
+      <c r="C22" s="7">
+        <v>858</v>
+      </c>
+      <c r="D22" s="9">
+        <v>965</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -769,13 +786,13 @@
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="1">
-        <v>747</v>
-      </c>
-      <c r="D23" s="1">
-        <v>751</v>
+        <v>4</v>
+      </c>
+      <c r="C23" s="7">
+        <v>859</v>
+      </c>
+      <c r="D23" s="9">
+        <v>967</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -783,307 +800,277 @@
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="1">
-        <v>747</v>
-      </c>
-      <c r="D24" s="1">
-        <v>746</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C24" s="2">
+        <v>860</v>
+      </c>
+      <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="1">
-        <v>746</v>
-      </c>
-      <c r="D25" s="1">
-        <v>750</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C25" s="3">
+        <v>1013</v>
+      </c>
+      <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C26" s="1">
-        <v>746</v>
+        <v>863</v>
       </c>
       <c r="D26" s="1">
-        <v>751</v>
+        <v>862</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C27" s="1">
-        <v>746</v>
-      </c>
-      <c r="D27" s="1">
-        <v>747</v>
+        <v>818</v>
+      </c>
+      <c r="D27" s="4">
+        <v>795</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="1">
-        <v>775</v>
-      </c>
-      <c r="D28" s="1">
-        <v>1073</v>
+        <v>0</v>
+      </c>
+      <c r="C28" s="4">
+        <v>824</v>
+      </c>
+      <c r="D28" s="4">
+        <v>796</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C29" s="1">
-        <v>748</v>
-      </c>
-      <c r="D29" s="1">
-        <v>1073</v>
+        <v>829</v>
+      </c>
+      <c r="D29" s="4">
+        <v>797</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C30" s="1">
-        <v>859</v>
-      </c>
-      <c r="D30" s="1">
-        <v>1073</v>
-      </c>
+        <v>833</v>
+      </c>
+      <c r="D30" s="4"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" s="2">
-        <v>860</v>
-      </c>
-      <c r="D31" s="1">
-        <v>1073</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C31" s="1">
+        <v>838</v>
+      </c>
+      <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" s="3">
-        <v>1013</v>
-      </c>
-      <c r="D32" s="1">
-        <v>1073</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C32" s="1">
+        <v>842</v>
+      </c>
+      <c r="D32" s="4"/>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C33" s="1">
-        <v>858</v>
-      </c>
-      <c r="D33" s="1">
-        <v>1073</v>
+        <v>812</v>
+      </c>
+      <c r="D33" s="4">
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C34" s="1">
-        <v>749</v>
-      </c>
-      <c r="D34" s="1">
-        <v>1073</v>
-      </c>
+        <v>821</v>
+      </c>
+      <c r="D34" s="4"/>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="3">
-        <v>748</v>
-      </c>
-      <c r="D35" s="1">
-        <v>1073</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C35" s="1">
+        <v>832</v>
+      </c>
+      <c r="D35" s="4"/>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C36" s="1">
-        <v>775</v>
-      </c>
-      <c r="D36" s="1">
-        <v>1074</v>
-      </c>
+        <v>836</v>
+      </c>
+      <c r="D36" s="4"/>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C37" s="1">
-        <v>748</v>
-      </c>
-      <c r="D37" s="1">
-        <v>1074</v>
-      </c>
+        <v>839</v>
+      </c>
+      <c r="D37" s="4"/>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C38" s="1">
-        <v>859</v>
-      </c>
-      <c r="D38" s="1">
-        <v>1074</v>
-      </c>
+        <v>848</v>
+      </c>
+      <c r="D38" s="4"/>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C39" s="2">
-        <v>860</v>
-      </c>
-      <c r="D39" s="1">
-        <v>1074</v>
+        <v>2</v>
+      </c>
+      <c r="C39" s="1">
+        <v>823</v>
+      </c>
+      <c r="D39" s="4">
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40" s="3">
-        <v>1013</v>
-      </c>
-      <c r="D40" s="1">
-        <v>1074</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C40" s="1">
+        <v>831</v>
+      </c>
+      <c r="D40" s="4"/>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C41" s="1">
-        <v>858</v>
-      </c>
-      <c r="D41" s="1">
-        <v>1074</v>
-      </c>
+        <v>835</v>
+      </c>
+      <c r="D41" s="4"/>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C42" s="1">
-        <v>749</v>
-      </c>
-      <c r="D42" s="1">
-        <v>1074</v>
-      </c>
+        <v>840</v>
+      </c>
+      <c r="D42" s="4"/>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C43" s="3">
-        <v>748</v>
-      </c>
-      <c r="D43" s="1">
-        <v>1074</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C43" s="1">
+        <v>843</v>
+      </c>
+      <c r="D43" s="4"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C44" s="1">
-        <v>863</v>
-      </c>
-      <c r="D44" s="1">
-        <v>862</v>
-      </c>
+        <v>820</v>
+      </c>
+      <c r="D44" s="4"/>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C45" s="1">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="D45" s="4">
-        <v>795</v>
+        <v>811</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1091,13 +1078,13 @@
         <v>7</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C46" s="4">
-        <v>824</v>
+        <v>3</v>
+      </c>
+      <c r="C46" s="1">
+        <v>822</v>
       </c>
       <c r="D46" s="4">
-        <v>796</v>
+        <v>810</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1105,13 +1092,13 @@
         <v>7</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C47" s="1">
-        <v>829</v>
+        <v>834</v>
       </c>
       <c r="D47" s="4">
-        <v>797</v>
+        <v>854</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1119,49 +1106,53 @@
         <v>7</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C48" s="1">
-        <v>833</v>
-      </c>
-      <c r="D48" s="4"/>
+        <v>841</v>
+      </c>
+      <c r="D48" s="4">
+        <v>855</v>
+      </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C49" s="1">
-        <v>838</v>
-      </c>
-      <c r="D49" s="4"/>
+        <v>830</v>
+      </c>
+      <c r="D49" s="4">
+        <v>797</v>
+      </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C50" s="1">
-        <v>842</v>
-      </c>
-      <c r="D50" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="C50" s="4">
+        <v>845</v>
+      </c>
+      <c r="D50" s="4">
+        <v>795</v>
+      </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C51" s="1">
-        <v>812</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C51" s="1"/>
       <c r="D51" s="4">
-        <v>25</v>
+        <v>804</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1169,73 +1160,71 @@
         <v>7</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C52" s="1">
-        <v>821</v>
-      </c>
-      <c r="D52" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="C52" s="1"/>
+      <c r="D52" s="4">
+        <v>805</v>
+      </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C53" s="1">
-        <v>832</v>
-      </c>
-      <c r="D53" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="C53" s="1"/>
+      <c r="D53" s="4">
+        <v>850</v>
+      </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C54" s="1">
-        <v>836</v>
-      </c>
-      <c r="D54" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="C54" s="1"/>
+      <c r="D54" s="4">
+        <v>851</v>
+      </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C55" s="1">
-        <v>839</v>
-      </c>
-      <c r="D55" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="C55" s="1"/>
+      <c r="D55" s="4">
+        <v>809</v>
+      </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C56" s="1">
-        <v>848</v>
-      </c>
-      <c r="D56" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="C56" s="1"/>
+      <c r="D56" s="4">
+        <v>852</v>
+      </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C57" s="1">
-        <v>823</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C57" s="1"/>
       <c r="D57" s="4">
-        <v>25</v>
+        <v>806</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1243,60 +1232,60 @@
         <v>7</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C58" s="1">
-        <v>831</v>
-      </c>
-      <c r="D58" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="C58" s="1"/>
+      <c r="D58" s="4">
+        <v>411</v>
+      </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C59" s="1">
-        <v>835</v>
-      </c>
-      <c r="D59" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="C59" s="1"/>
+      <c r="D59" s="4">
+        <v>463</v>
+      </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C60" s="1">
-        <v>840</v>
-      </c>
-      <c r="D60" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="C60" s="1"/>
+      <c r="D60" s="4">
+        <v>19</v>
+      </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C61" s="1">
-        <v>843</v>
-      </c>
-      <c r="D61" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="C61" s="1"/>
+      <c r="D61" s="4">
+        <v>507</v>
+      </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C62" s="1">
-        <v>820</v>
-      </c>
-      <c r="D62" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="C62" s="1"/>
+      <c r="D62" s="4">
+        <v>765</v>
+      </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="1" t="s">
@@ -1305,11 +1294,9 @@
       <c r="B63" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C63" s="1">
-        <v>819</v>
-      </c>
+      <c r="C63" s="1"/>
       <c r="D63" s="4">
-        <v>811</v>
+        <v>766</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1319,11 +1306,9 @@
       <c r="B64" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C64" s="1">
-        <v>822</v>
-      </c>
+      <c r="C64" s="1"/>
       <c r="D64" s="4">
-        <v>810</v>
+        <v>934</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1333,11 +1318,9 @@
       <c r="B65" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C65" s="1">
-        <v>834</v>
-      </c>
+      <c r="C65" s="1"/>
       <c r="D65" s="4">
-        <v>854</v>
+        <v>938</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1347,11 +1330,9 @@
       <c r="B66" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C66" s="1">
-        <v>841</v>
-      </c>
+      <c r="C66" s="1"/>
       <c r="D66" s="4">
-        <v>855</v>
+        <v>513</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1361,11 +1342,9 @@
       <c r="B67" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C67" s="1">
-        <v>830</v>
-      </c>
+      <c r="C67" s="1"/>
       <c r="D67" s="4">
-        <v>797</v>
+        <v>405</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1375,11 +1354,9 @@
       <c r="B68" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C68" s="4">
-        <v>845</v>
-      </c>
+      <c r="C68" s="1"/>
       <c r="D68" s="4">
-        <v>795</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -1391,7 +1368,7 @@
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="4">
-        <v>804</v>
+        <v>362</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1403,7 +1380,7 @@
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="4">
-        <v>805</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1415,7 +1392,7 @@
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="4">
-        <v>850</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1427,7 +1404,7 @@
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="4">
-        <v>851</v>
+        <v>808</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1439,7 +1416,7 @@
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="4">
-        <v>809</v>
+        <v>807</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1451,7 +1428,7 @@
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="4">
-        <v>852</v>
+        <v>410</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -1463,223 +1440,247 @@
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="4">
-        <v>806</v>
+        <v>861</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C76" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="C76" s="1">
+        <v>865</v>
+      </c>
       <c r="D76" s="4">
-        <v>411</v>
+        <v>965</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C77" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="C77" s="1">
+        <v>866</v>
+      </c>
       <c r="D77" s="4">
-        <v>463</v>
+        <v>967</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C78" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="C78" s="1">
+        <v>867</v>
+      </c>
       <c r="D78" s="4">
-        <v>19</v>
+        <v>970</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C79" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="C79" s="1">
+        <v>868</v>
+      </c>
       <c r="D79" s="4">
-        <v>507</v>
+        <v>938</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C80" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="C80" s="1">
+        <v>869</v>
+      </c>
       <c r="D80" s="4">
-        <v>765</v>
+        <v>934</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C81" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="C81" s="1">
+        <v>870</v>
+      </c>
       <c r="D81" s="4">
-        <v>766</v>
+        <v>513</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C82" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="C82" s="1">
+        <v>871</v>
+      </c>
       <c r="D82" s="4">
-        <v>934</v>
+        <v>405</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C83" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="C83" s="1">
+        <v>872</v>
+      </c>
       <c r="D83" s="4">
-        <v>938</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C84" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="C84" s="1">
+        <v>873</v>
+      </c>
       <c r="D84" s="4">
-        <v>513</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C85" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="C85" s="1">
+        <v>874</v>
+      </c>
       <c r="D85" s="4">
-        <v>405</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C86" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="C86" s="1">
+        <v>875</v>
+      </c>
       <c r="D86" s="4">
-        <v>1081</v>
+        <v>19</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C87" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="C87" s="1">
+        <v>876</v>
+      </c>
       <c r="D87" s="4">
-        <v>362</v>
+        <v>507</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C88" s="1"/>
       <c r="D88" s="4">
-        <v>1088</v>
+        <v>410</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C89" s="1"/>
       <c r="D89" s="4">
-        <v>1090</v>
+        <v>411</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C90" s="1"/>
       <c r="D90" s="4">
-        <v>808</v>
+        <v>463</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C91" s="1"/>
       <c r="D91" s="4">
-        <v>807</v>
+        <v>362</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C92" s="1"/>
       <c r="D92" s="4">
-        <v>410</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C93" s="1"/>
       <c r="D93" s="4">
-        <v>861</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -1687,13 +1688,13 @@
         <v>8</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C94" s="1">
-        <v>865</v>
+        <v>1106</v>
       </c>
       <c r="D94" s="4">
-        <v>965</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -1701,13 +1702,13 @@
         <v>8</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C95" s="1">
-        <v>866</v>
-      </c>
-      <c r="D95" s="4">
-        <v>967</v>
+        <v>1103</v>
+      </c>
+      <c r="D95" s="1">
+        <v>1089</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -1715,374 +1716,374 @@
         <v>8</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C96" s="1">
-        <v>867</v>
-      </c>
-      <c r="D96" s="4">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4">
+        <v>1102</v>
+      </c>
+      <c r="D96" s="1"/>
+    </row>
+    <row r="97" spans="1:5">
       <c r="A97" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C97" s="1">
-        <v>868</v>
-      </c>
-      <c r="D97" s="4">
-        <v>938</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4">
+        <v>1101</v>
+      </c>
+      <c r="D97" s="1"/>
+    </row>
+    <row r="98" spans="1:5">
       <c r="A98" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C98" s="1">
-        <v>869</v>
-      </c>
-      <c r="D98" s="4">
-        <v>934</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4">
+        <v>1100</v>
+      </c>
+      <c r="D98" s="1"/>
+    </row>
+    <row r="99" spans="1:5">
       <c r="A99" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C99" s="1">
-        <v>870</v>
-      </c>
-      <c r="D99" s="4">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4">
+        <v>1099</v>
+      </c>
+      <c r="D99" s="1"/>
+    </row>
+    <row r="100" spans="1:5">
       <c r="A100" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C100" s="1">
-        <v>871</v>
-      </c>
-      <c r="D100" s="4">
+        <v>1098</v>
+      </c>
+      <c r="D100" s="1"/>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C101" s="1">
+        <v>1097</v>
+      </c>
+      <c r="D101" s="1"/>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C102" s="1">
+        <v>1096</v>
+      </c>
+      <c r="D102" s="1"/>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C103" s="1">
+        <v>1095</v>
+      </c>
+      <c r="D103" s="1"/>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C104" s="1">
+        <v>1094</v>
+      </c>
+      <c r="D104" s="1"/>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C105" s="1">
+        <v>1093</v>
+      </c>
+      <c r="D105" s="1"/>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" t="s">
+        <v>13</v>
+      </c>
+      <c r="B106" t="s">
+        <v>0</v>
+      </c>
+      <c r="C106" s="7">
+        <v>723</v>
+      </c>
+      <c r="D106" s="7">
+        <v>24</v>
+      </c>
+      <c r="E106" s="7"/>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C107" s="7">
+        <v>716</v>
+      </c>
+      <c r="D107" s="7">
+        <v>707</v>
+      </c>
+      <c r="E107" s="7"/>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C108" s="7">
+        <v>1081</v>
+      </c>
+      <c r="D108" s="7">
+        <v>347</v>
+      </c>
+      <c r="E108" s="7"/>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C109" s="7">
         <v>405</v>
       </c>
-    </row>
-    <row r="101" spans="1:4">
-      <c r="A101" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C101" s="1">
-        <v>872</v>
-      </c>
-      <c r="D101" s="4">
-        <v>1081</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4">
-      <c r="A102" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C102" s="1">
-        <v>873</v>
-      </c>
-      <c r="D102" s="4">
-        <v>1088</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4">
-      <c r="A103" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C103" s="1">
-        <v>874</v>
-      </c>
-      <c r="D103" s="4">
-        <v>1090</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4">
-      <c r="A104" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C104" s="1">
-        <v>875</v>
-      </c>
-      <c r="D104" s="4">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4">
-      <c r="A105" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C105" s="1">
-        <v>876</v>
-      </c>
-      <c r="D105" s="4">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4">
-      <c r="A106" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C106" s="1"/>
-      <c r="D106" s="4">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4">
-      <c r="A107" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C107" s="1"/>
-      <c r="D107" s="4">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4">
-      <c r="A108" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C108" s="1"/>
-      <c r="D108" s="4">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4">
-      <c r="A109" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C109" s="1"/>
-      <c r="D109" s="4">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4">
-      <c r="A110" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C110" s="1"/>
-      <c r="D110" s="4">
-        <v>1104</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4">
-      <c r="A111" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C111" s="1"/>
-      <c r="D111" s="4">
-        <v>1105</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4">
-      <c r="A112" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C112" s="1">
-        <v>1106</v>
-      </c>
-      <c r="D112" s="4">
-        <v>1081</v>
-      </c>
+      <c r="D109" s="6">
+        <v>346</v>
+      </c>
+      <c r="E109" s="7"/>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C110" s="7">
+        <v>251</v>
+      </c>
+      <c r="D110" s="6"/>
+      <c r="E110" s="7"/>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C111" s="7">
+        <v>735</v>
+      </c>
+      <c r="D111" s="6"/>
+      <c r="E111" s="7"/>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C112" s="7">
+        <v>729</v>
+      </c>
+      <c r="D112" s="6"/>
+      <c r="E112" s="7"/>
     </row>
     <row r="113" spans="1:5">
-      <c r="A113" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C113" s="1">
-        <v>1103</v>
-      </c>
-      <c r="D113" s="1">
-        <v>1089</v>
-      </c>
+      <c r="A113" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C113" s="7">
+        <v>862</v>
+      </c>
+      <c r="D113" s="6"/>
+      <c r="E113" s="7"/>
     </row>
     <row r="114" spans="1:5">
-      <c r="A114" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C114" s="1">
-        <v>1102</v>
-      </c>
-      <c r="D114" s="1"/>
+      <c r="A114" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C114" s="7">
+        <v>1013</v>
+      </c>
+      <c r="D114" s="6"/>
+      <c r="E114" s="7"/>
     </row>
     <row r="115" spans="1:5">
-      <c r="A115" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C115" s="1">
-        <v>1101</v>
-      </c>
-      <c r="D115" s="1"/>
+      <c r="A115" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C115" s="7">
+        <v>334</v>
+      </c>
+      <c r="D115" s="6"/>
+      <c r="E115" s="7"/>
     </row>
     <row r="116" spans="1:5">
-      <c r="A116" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C116" s="1">
-        <v>1100</v>
-      </c>
-      <c r="D116" s="1"/>
+      <c r="A116" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C116" s="7">
+        <v>989</v>
+      </c>
+      <c r="D116" s="6"/>
+      <c r="E116" s="7"/>
     </row>
     <row r="117" spans="1:5">
-      <c r="A117" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C117" s="1">
-        <v>1099</v>
-      </c>
-      <c r="D117" s="1"/>
+      <c r="A117" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C117" s="7">
+        <v>923</v>
+      </c>
+      <c r="D117" s="6"/>
+      <c r="E117" s="7"/>
     </row>
     <row r="118" spans="1:5">
-      <c r="A118" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C118" s="1">
-        <v>1098</v>
-      </c>
-      <c r="D118" s="1"/>
+      <c r="A118" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C118" s="7">
+        <v>1027</v>
+      </c>
+      <c r="D118" s="6"/>
+      <c r="E118" s="7"/>
     </row>
     <row r="119" spans="1:5">
-      <c r="A119" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C119" s="1">
-        <v>1097</v>
-      </c>
-      <c r="D119" s="1"/>
+      <c r="A119" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C119" s="7">
+        <v>710</v>
+      </c>
+      <c r="D119" s="6"/>
+      <c r="E119" s="7"/>
     </row>
     <row r="120" spans="1:5">
-      <c r="A120" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C120" s="1">
-        <v>1096</v>
-      </c>
-      <c r="D120" s="1"/>
+      <c r="A120" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C120" s="7">
+        <v>1031</v>
+      </c>
+      <c r="D120" s="6"/>
+      <c r="E120" s="7"/>
     </row>
     <row r="121" spans="1:5">
-      <c r="A121" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C121" s="1">
-        <v>1095</v>
-      </c>
-      <c r="D121" s="1"/>
+      <c r="A121" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C121" s="7">
+        <v>859</v>
+      </c>
+      <c r="D121" s="6"/>
+      <c r="E121" s="7"/>
     </row>
     <row r="122" spans="1:5">
-      <c r="A122" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C122" s="1">
-        <v>1094</v>
-      </c>
-      <c r="D122" s="1"/>
+      <c r="A122" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C122" s="7">
+        <v>1007</v>
+      </c>
+      <c r="D122" s="6"/>
+      <c r="E122" s="7"/>
     </row>
     <row r="123" spans="1:5">
-      <c r="A123" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C123" s="1">
-        <v>1093</v>
-      </c>
-      <c r="D123" s="1"/>
+      <c r="A123" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B123" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C123" s="7">
+        <v>770</v>
+      </c>
+      <c r="D123" s="6"/>
+      <c r="E123" s="7"/>
     </row>
     <row r="124" spans="1:5">
-      <c r="A124" t="s">
-        <v>13</v>
-      </c>
-      <c r="B124" t="s">
+      <c r="A124" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B124" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C124" s="7">
-        <v>723</v>
-      </c>
-      <c r="D124" s="7">
-        <v>24</v>
-      </c>
+        <v>667</v>
+      </c>
+      <c r="D124" s="6"/>
       <c r="E124" s="7"/>
     </row>
     <row r="125" spans="1:5">
@@ -2093,11 +2094,9 @@
         <v>0</v>
       </c>
       <c r="C125" s="7">
-        <v>716</v>
-      </c>
-      <c r="D125" s="7">
-        <v>707</v>
-      </c>
+        <v>934</v>
+      </c>
+      <c r="D125" s="6"/>
       <c r="E125" s="7"/>
     </row>
     <row r="126" spans="1:5">
@@ -2108,11 +2107,9 @@
         <v>0</v>
       </c>
       <c r="C126" s="7">
-        <v>1081</v>
-      </c>
-      <c r="D126" s="7">
-        <v>347</v>
-      </c>
+        <v>1087</v>
+      </c>
+      <c r="D126" s="6"/>
       <c r="E126" s="7"/>
     </row>
     <row r="127" spans="1:5">
@@ -2123,11 +2120,9 @@
         <v>0</v>
       </c>
       <c r="C127" s="7">
-        <v>405</v>
-      </c>
-      <c r="D127" s="6">
-        <v>346</v>
-      </c>
+        <v>715</v>
+      </c>
+      <c r="D127" s="6"/>
       <c r="E127" s="7"/>
     </row>
     <row r="128" spans="1:5">
@@ -2138,7 +2133,7 @@
         <v>0</v>
       </c>
       <c r="C128" s="7">
-        <v>251</v>
+        <v>1083</v>
       </c>
       <c r="D128" s="6"/>
       <c r="E128" s="7"/>
@@ -2151,7 +2146,7 @@
         <v>0</v>
       </c>
       <c r="C129" s="7">
-        <v>735</v>
+        <v>745</v>
       </c>
       <c r="D129" s="6"/>
       <c r="E129" s="7"/>
@@ -2164,7 +2159,7 @@
         <v>0</v>
       </c>
       <c r="C130" s="7">
-        <v>729</v>
+        <v>765</v>
       </c>
       <c r="D130" s="6"/>
       <c r="E130" s="7"/>
@@ -2177,7 +2172,7 @@
         <v>0</v>
       </c>
       <c r="C131" s="7">
-        <v>862</v>
+        <v>1020</v>
       </c>
       <c r="D131" s="6"/>
       <c r="E131" s="7"/>
@@ -2190,7 +2185,7 @@
         <v>0</v>
       </c>
       <c r="C132" s="7">
-        <v>1013</v>
+        <v>1029</v>
       </c>
       <c r="D132" s="6"/>
       <c r="E132" s="7"/>
@@ -2203,7 +2198,7 @@
         <v>0</v>
       </c>
       <c r="C133" s="7">
-        <v>334</v>
+        <v>1011</v>
       </c>
       <c r="D133" s="6"/>
       <c r="E133" s="7"/>
@@ -2216,7 +2211,7 @@
         <v>0</v>
       </c>
       <c r="C134" s="7">
-        <v>989</v>
+        <v>1026</v>
       </c>
       <c r="D134" s="6"/>
       <c r="E134" s="7"/>
@@ -2229,7 +2224,7 @@
         <v>0</v>
       </c>
       <c r="C135" s="7">
-        <v>923</v>
+        <v>919</v>
       </c>
       <c r="D135" s="6"/>
       <c r="E135" s="7"/>
@@ -2242,7 +2237,7 @@
         <v>0</v>
       </c>
       <c r="C136" s="7">
-        <v>1027</v>
+        <v>749</v>
       </c>
       <c r="D136" s="6"/>
       <c r="E136" s="7"/>
@@ -2255,7 +2250,7 @@
         <v>0</v>
       </c>
       <c r="C137" s="7">
-        <v>710</v>
+        <v>1030</v>
       </c>
       <c r="D137" s="6"/>
       <c r="E137" s="7"/>
@@ -2268,7 +2263,7 @@
         <v>0</v>
       </c>
       <c r="C138" s="7">
-        <v>1031</v>
+        <v>748</v>
       </c>
       <c r="D138" s="6"/>
       <c r="E138" s="7"/>
@@ -2281,7 +2276,7 @@
         <v>0</v>
       </c>
       <c r="C139" s="7">
-        <v>859</v>
+        <v>744</v>
       </c>
       <c r="D139" s="6"/>
       <c r="E139" s="7"/>
@@ -2294,7 +2289,7 @@
         <v>0</v>
       </c>
       <c r="C140" s="7">
-        <v>1007</v>
+        <v>1003</v>
       </c>
       <c r="D140" s="6"/>
       <c r="E140" s="7"/>
@@ -2307,7 +2302,7 @@
         <v>0</v>
       </c>
       <c r="C141" s="7">
-        <v>770</v>
+        <v>43</v>
       </c>
       <c r="D141" s="6"/>
       <c r="E141" s="7"/>
@@ -2320,7 +2315,7 @@
         <v>0</v>
       </c>
       <c r="C142" s="7">
-        <v>667</v>
+        <v>858</v>
       </c>
       <c r="D142" s="6"/>
       <c r="E142" s="7"/>
@@ -2333,7 +2328,7 @@
         <v>0</v>
       </c>
       <c r="C143" s="7">
-        <v>934</v>
+        <v>766</v>
       </c>
       <c r="D143" s="6"/>
       <c r="E143" s="7"/>
@@ -2346,7 +2341,7 @@
         <v>0</v>
       </c>
       <c r="C144" s="7">
-        <v>1087</v>
+        <v>767</v>
       </c>
       <c r="D144" s="6"/>
       <c r="E144" s="7"/>
@@ -2359,7 +2354,7 @@
         <v>0</v>
       </c>
       <c r="C145" s="7">
-        <v>715</v>
+        <v>769</v>
       </c>
       <c r="D145" s="6"/>
       <c r="E145" s="7"/>
@@ -2372,7 +2367,7 @@
         <v>0</v>
       </c>
       <c r="C146" s="7">
-        <v>1083</v>
+        <v>892</v>
       </c>
       <c r="D146" s="6"/>
       <c r="E146" s="7"/>
@@ -2385,7 +2380,7 @@
         <v>0</v>
       </c>
       <c r="C147" s="7">
-        <v>745</v>
+        <v>119</v>
       </c>
       <c r="D147" s="6"/>
       <c r="E147" s="7"/>
@@ -2398,7 +2393,7 @@
         <v>0</v>
       </c>
       <c r="C148" s="7">
-        <v>765</v>
+        <v>920</v>
       </c>
       <c r="D148" s="6"/>
       <c r="E148" s="7"/>
@@ -2411,7 +2406,7 @@
         <v>0</v>
       </c>
       <c r="C149" s="7">
-        <v>1020</v>
+        <v>956</v>
       </c>
       <c r="D149" s="6"/>
       <c r="E149" s="7"/>
@@ -2424,7 +2419,7 @@
         <v>0</v>
       </c>
       <c r="C150" s="7">
-        <v>1029</v>
+        <v>1009</v>
       </c>
       <c r="D150" s="6"/>
       <c r="E150" s="7"/>
@@ -2437,7 +2432,7 @@
         <v>0</v>
       </c>
       <c r="C151" s="7">
-        <v>1011</v>
+        <v>30</v>
       </c>
       <c r="D151" s="6"/>
       <c r="E151" s="7"/>
@@ -2450,7 +2445,7 @@
         <v>0</v>
       </c>
       <c r="C152" s="7">
-        <v>1026</v>
+        <v>957</v>
       </c>
       <c r="D152" s="6"/>
       <c r="E152" s="7"/>
@@ -2463,7 +2458,7 @@
         <v>0</v>
       </c>
       <c r="C153" s="7">
-        <v>919</v>
+        <v>860</v>
       </c>
       <c r="D153" s="6"/>
       <c r="E153" s="7"/>
@@ -2476,247 +2471,13 @@
         <v>0</v>
       </c>
       <c r="C154" s="7">
-        <v>749</v>
+        <v>1028</v>
       </c>
       <c r="D154" s="6"/>
       <c r="E154" s="7"/>
     </row>
-    <row r="155" spans="1:5">
-      <c r="A155" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B155" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C155" s="7">
-        <v>1030</v>
-      </c>
-      <c r="D155" s="6"/>
-      <c r="E155" s="7"/>
-    </row>
-    <row r="156" spans="1:5">
-      <c r="A156" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B156" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C156" s="7">
-        <v>748</v>
-      </c>
-      <c r="D156" s="6"/>
-      <c r="E156" s="7"/>
-    </row>
-    <row r="157" spans="1:5">
-      <c r="A157" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B157" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C157" s="7">
-        <v>744</v>
-      </c>
-      <c r="D157" s="6"/>
-      <c r="E157" s="7"/>
-    </row>
-    <row r="158" spans="1:5">
-      <c r="A158" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B158" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C158" s="7">
-        <v>1003</v>
-      </c>
-      <c r="D158" s="6"/>
-      <c r="E158" s="7"/>
-    </row>
-    <row r="159" spans="1:5">
-      <c r="A159" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B159" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C159" s="7">
-        <v>43</v>
-      </c>
-      <c r="D159" s="6"/>
-      <c r="E159" s="7"/>
-    </row>
-    <row r="160" spans="1:5">
-      <c r="A160" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B160" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C160" s="7">
-        <v>858</v>
-      </c>
-      <c r="D160" s="6"/>
-      <c r="E160" s="7"/>
-    </row>
-    <row r="161" spans="1:5">
-      <c r="A161" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B161" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C161" s="7">
-        <v>766</v>
-      </c>
-      <c r="D161" s="6"/>
-      <c r="E161" s="7"/>
-    </row>
-    <row r="162" spans="1:5">
-      <c r="A162" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B162" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C162" s="7">
-        <v>767</v>
-      </c>
-      <c r="D162" s="6"/>
-      <c r="E162" s="7"/>
-    </row>
-    <row r="163" spans="1:5">
-      <c r="A163" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B163" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C163" s="7">
-        <v>769</v>
-      </c>
-      <c r="D163" s="6"/>
-      <c r="E163" s="7"/>
-    </row>
-    <row r="164" spans="1:5">
-      <c r="A164" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B164" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C164" s="7">
-        <v>892</v>
-      </c>
-      <c r="D164" s="6"/>
-      <c r="E164" s="7"/>
-    </row>
-    <row r="165" spans="1:5">
-      <c r="A165" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B165" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C165" s="7">
-        <v>119</v>
-      </c>
-      <c r="D165" s="6"/>
-      <c r="E165" s="7"/>
-    </row>
-    <row r="166" spans="1:5">
-      <c r="A166" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B166" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C166" s="7">
-        <v>920</v>
-      </c>
-      <c r="D166" s="6"/>
-      <c r="E166" s="7"/>
-    </row>
-    <row r="167" spans="1:5">
-      <c r="A167" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B167" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C167" s="7">
-        <v>956</v>
-      </c>
-      <c r="D167" s="6"/>
-      <c r="E167" s="7"/>
-    </row>
-    <row r="168" spans="1:5">
-      <c r="A168" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B168" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C168" s="7">
-        <v>1009</v>
-      </c>
-      <c r="D168" s="6"/>
-      <c r="E168" s="7"/>
-    </row>
-    <row r="169" spans="1:5">
-      <c r="A169" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B169" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C169" s="7">
-        <v>30</v>
-      </c>
-      <c r="D169" s="6"/>
-      <c r="E169" s="7"/>
-    </row>
-    <row r="170" spans="1:5">
-      <c r="A170" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B170" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C170" s="7">
-        <v>957</v>
-      </c>
-      <c r="D170" s="6"/>
-      <c r="E170" s="7"/>
-    </row>
-    <row r="171" spans="1:5">
-      <c r="A171" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B171" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C171" s="7">
-        <v>860</v>
-      </c>
-      <c r="D171" s="6"/>
-      <c r="E171" s="7"/>
-    </row>
-    <row r="172" spans="1:5">
-      <c r="A172" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B172" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C172" s="7">
-        <v>1028</v>
-      </c>
-      <c r="D172" s="6"/>
-      <c r="E172" s="7"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:D172">
+  <autoFilter ref="A1:D154">
     <sortState ref="A45:D95">
       <sortCondition ref="A1:A174"/>
     </sortState>
@@ -2724,4 +2485,52 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="7">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="7">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="7">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="7">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="2">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="3">
+        <v>1013</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:A16">
+    <sortCondition ref="A1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixes to issues with Evans definitions
</commit_message>
<xml_diff>
--- a/analysis_specifications/analysis2InputSpecifications.xlsx
+++ b/analysis_specifications/analysis2InputSpecifications.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$143</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$146</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="14">
   <si>
     <t>a</t>
   </si>
@@ -462,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E144"/>
+  <dimension ref="A1:E147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1278,43 +1278,38 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C64" s="1">
-        <v>1093</v>
-      </c>
-      <c r="D64" s="7">
-        <v>1089</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C65" s="1">
-        <v>1094</v>
-      </c>
-      <c r="D65" s="7"/>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C66" s="1">
-        <v>1095</v>
-      </c>
-      <c r="D66" s="7"/>
+    <row r="64" spans="1:4" s="7" customFormat="1">
+      <c r="A64" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D64" s="4">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" s="7" customFormat="1">
+      <c r="A65" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D65" s="4">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" s="7" customFormat="1">
+      <c r="A66" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D66" s="4">
+        <v>1104</v>
+      </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="1" t="s">
@@ -1324,9 +1319,11 @@
         <v>1</v>
       </c>
       <c r="C67" s="1">
-        <v>1096</v>
-      </c>
-      <c r="D67" s="7"/>
+        <v>1093</v>
+      </c>
+      <c r="D67" s="7">
+        <v>1089</v>
+      </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="1" t="s">
@@ -1336,7 +1333,7 @@
         <v>1</v>
       </c>
       <c r="C68" s="1">
-        <v>1097</v>
+        <v>1094</v>
       </c>
       <c r="D68" s="7"/>
     </row>
@@ -1348,7 +1345,7 @@
         <v>1</v>
       </c>
       <c r="C69" s="1">
-        <v>1098</v>
+        <v>1095</v>
       </c>
       <c r="D69" s="7"/>
     </row>
@@ -1360,7 +1357,7 @@
         <v>1</v>
       </c>
       <c r="C70" s="1">
-        <v>1099</v>
+        <v>1096</v>
       </c>
       <c r="D70" s="7"/>
     </row>
@@ -1372,7 +1369,7 @@
         <v>1</v>
       </c>
       <c r="C71" s="1">
-        <v>1100</v>
+        <v>1097</v>
       </c>
       <c r="D71" s="7"/>
     </row>
@@ -1384,7 +1381,7 @@
         <v>1</v>
       </c>
       <c r="C72" s="1">
-        <v>1101</v>
+        <v>1098</v>
       </c>
       <c r="D72" s="7"/>
     </row>
@@ -1396,7 +1393,7 @@
         <v>1</v>
       </c>
       <c r="C73" s="1">
-        <v>1102</v>
+        <v>1099</v>
       </c>
       <c r="D73" s="7"/>
     </row>
@@ -1408,7 +1405,7 @@
         <v>1</v>
       </c>
       <c r="C74" s="1">
-        <v>1103</v>
+        <v>1100</v>
       </c>
       <c r="D74" s="7"/>
     </row>
@@ -1420,49 +1417,43 @@
         <v>1</v>
       </c>
       <c r="C75" s="1">
-        <v>1106</v>
-      </c>
+        <v>1101</v>
+      </c>
+      <c r="D75" s="7"/>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C76" s="1">
-        <v>30</v>
-      </c>
-      <c r="D76" s="7">
-        <v>1150</v>
-      </c>
+        <v>1102</v>
+      </c>
+      <c r="D76" s="7"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C77" s="1">
-        <v>119</v>
-      </c>
-      <c r="D77" s="7">
-        <v>707</v>
-      </c>
+        <v>1103</v>
+      </c>
+      <c r="D77" s="7"/>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C78" s="1">
-        <v>251</v>
-      </c>
-      <c r="D78" s="7">
-        <v>24</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -1473,10 +1464,10 @@
         <v>0</v>
       </c>
       <c r="C79" s="1">
-        <v>334</v>
-      </c>
-      <c r="D79" s="6">
-        <v>346</v>
+        <v>30</v>
+      </c>
+      <c r="D79" s="7">
+        <v>1150</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1487,7 +1478,10 @@
         <v>0</v>
       </c>
       <c r="C80" s="1">
-        <v>405</v>
+        <v>119</v>
+      </c>
+      <c r="D80" s="7">
+        <v>707</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -1498,9 +1492,11 @@
         <v>0</v>
       </c>
       <c r="C81" s="1">
-        <v>710</v>
-      </c>
-      <c r="D81" s="7"/>
+        <v>251</v>
+      </c>
+      <c r="D81" s="7">
+        <v>24</v>
+      </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="1" t="s">
@@ -1510,9 +1506,11 @@
         <v>0</v>
       </c>
       <c r="C82" s="1">
-        <v>715</v>
-      </c>
-      <c r="D82" s="7"/>
+        <v>334</v>
+      </c>
+      <c r="D82" s="6">
+        <v>346</v>
+      </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="1" t="s">
@@ -1522,7 +1520,7 @@
         <v>0</v>
       </c>
       <c r="C83" s="1">
-        <v>716</v>
+        <v>405</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -1533,8 +1531,9 @@
         <v>0</v>
       </c>
       <c r="C84" s="1">
-        <v>723</v>
-      </c>
+        <v>710</v>
+      </c>
+      <c r="D84" s="7"/>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="1" t="s">
@@ -1544,7 +1543,7 @@
         <v>0</v>
       </c>
       <c r="C85" s="1">
-        <v>729</v>
+        <v>715</v>
       </c>
       <c r="D85" s="7"/>
     </row>
@@ -1556,9 +1555,8 @@
         <v>0</v>
       </c>
       <c r="C86" s="1">
-        <v>735</v>
-      </c>
-      <c r="D86" s="7"/>
+        <v>716</v>
+      </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="1" t="s">
@@ -1568,9 +1566,8 @@
         <v>0</v>
       </c>
       <c r="C87" s="1">
-        <v>744</v>
-      </c>
-      <c r="D87" s="7"/>
+        <v>723</v>
+      </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="1" t="s">
@@ -1580,9 +1577,9 @@
         <v>0</v>
       </c>
       <c r="C88" s="1">
-        <v>745</v>
-      </c>
-      <c r="D88" s="1"/>
+        <v>729</v>
+      </c>
+      <c r="D88" s="7"/>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="1" t="s">
@@ -1592,8 +1589,9 @@
         <v>0</v>
       </c>
       <c r="C89" s="1">
-        <v>748</v>
-      </c>
+        <v>735</v>
+      </c>
+      <c r="D89" s="7"/>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="1" t="s">
@@ -1603,9 +1601,9 @@
         <v>0</v>
       </c>
       <c r="C90" s="1">
-        <v>749</v>
-      </c>
-      <c r="D90" s="1"/>
+        <v>744</v>
+      </c>
+      <c r="D90" s="7"/>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="1" t="s">
@@ -1615,7 +1613,7 @@
         <v>0</v>
       </c>
       <c r="C91" s="1">
-        <v>765</v>
+        <v>745</v>
       </c>
       <c r="D91" s="1"/>
     </row>
@@ -1627,9 +1625,8 @@
         <v>0</v>
       </c>
       <c r="C92" s="1">
-        <v>766</v>
-      </c>
-      <c r="D92" s="1"/>
+        <v>748</v>
+      </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="1" t="s">
@@ -1639,7 +1636,7 @@
         <v>0</v>
       </c>
       <c r="C93" s="1">
-        <v>767</v>
+        <v>749</v>
       </c>
       <c r="D93" s="1"/>
     </row>
@@ -1651,7 +1648,7 @@
         <v>0</v>
       </c>
       <c r="C94" s="1">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="D94" s="1"/>
     </row>
@@ -1663,7 +1660,7 @@
         <v>0</v>
       </c>
       <c r="C95" s="1">
-        <v>770</v>
+        <v>766</v>
       </c>
       <c r="D95" s="1"/>
     </row>
@@ -1675,7 +1672,7 @@
         <v>0</v>
       </c>
       <c r="C96" s="1">
-        <v>858</v>
+        <v>767</v>
       </c>
       <c r="D96" s="1"/>
     </row>
@@ -1687,7 +1684,7 @@
         <v>0</v>
       </c>
       <c r="C97" s="1">
-        <v>859</v>
+        <v>769</v>
       </c>
       <c r="D97" s="1"/>
     </row>
@@ -1699,60 +1696,57 @@
         <v>0</v>
       </c>
       <c r="C98" s="1">
+        <v>770</v>
+      </c>
+      <c r="D98" s="1"/>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C99" s="1">
+        <v>858</v>
+      </c>
+      <c r="D99" s="1"/>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C100" s="1">
+        <v>859</v>
+      </c>
+      <c r="D100" s="1"/>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C101" s="1">
         <v>860</v>
       </c>
-      <c r="D98" s="1"/>
-    </row>
-    <row r="99" spans="1:5">
-      <c r="A99" t="s">
-        <v>13</v>
-      </c>
-      <c r="B99" t="s">
-        <v>0</v>
-      </c>
-      <c r="C99" s="7">
+      <c r="D101" s="1"/>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" t="s">
+        <v>13</v>
+      </c>
+      <c r="B102" t="s">
+        <v>0</v>
+      </c>
+      <c r="C102" s="7">
         <v>862</v>
       </c>
-      <c r="D99" s="7"/>
-      <c r="E99" s="7"/>
-    </row>
-    <row r="100" spans="1:5">
-      <c r="A100" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B100" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C100" s="7">
-        <v>919</v>
-      </c>
-      <c r="D100" s="7"/>
-      <c r="E100" s="7"/>
-    </row>
-    <row r="101" spans="1:5">
-      <c r="A101" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B101" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C101" s="7">
-        <v>923</v>
-      </c>
-      <c r="D101" s="6"/>
-      <c r="E101" s="7"/>
-    </row>
-    <row r="102" spans="1:5">
-      <c r="A102" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B102" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C102" s="7">
-        <v>934</v>
-      </c>
-      <c r="D102" s="6"/>
+      <c r="D102" s="7"/>
       <c r="E102" s="7"/>
     </row>
     <row r="103" spans="1:5">
@@ -1763,9 +1757,9 @@
         <v>0</v>
       </c>
       <c r="C103" s="7">
-        <v>957</v>
-      </c>
-      <c r="D103" s="6"/>
+        <v>919</v>
+      </c>
+      <c r="D103" s="7"/>
       <c r="E103" s="7"/>
     </row>
     <row r="104" spans="1:5">
@@ -1776,7 +1770,7 @@
         <v>0</v>
       </c>
       <c r="C104" s="7">
-        <v>989</v>
+        <v>923</v>
       </c>
       <c r="D104" s="6"/>
       <c r="E104" s="7"/>
@@ -1789,7 +1783,7 @@
         <v>0</v>
       </c>
       <c r="C105" s="7">
-        <v>1003</v>
+        <v>934</v>
       </c>
       <c r="D105" s="6"/>
       <c r="E105" s="7"/>
@@ -1802,7 +1796,7 @@
         <v>0</v>
       </c>
       <c r="C106" s="7">
-        <v>1007</v>
+        <v>957</v>
       </c>
       <c r="D106" s="6"/>
       <c r="E106" s="7"/>
@@ -1815,7 +1809,7 @@
         <v>0</v>
       </c>
       <c r="C107" s="7">
-        <v>1009</v>
+        <v>989</v>
       </c>
       <c r="D107" s="6"/>
       <c r="E107" s="7"/>
@@ -1828,7 +1822,7 @@
         <v>0</v>
       </c>
       <c r="C108" s="7">
-        <v>1011</v>
+        <v>1003</v>
       </c>
       <c r="D108" s="6"/>
       <c r="E108" s="7"/>
@@ -1841,7 +1835,7 @@
         <v>0</v>
       </c>
       <c r="C109" s="7">
-        <v>1013</v>
+        <v>1007</v>
       </c>
       <c r="D109" s="6"/>
       <c r="E109" s="7"/>
@@ -1854,7 +1848,7 @@
         <v>0</v>
       </c>
       <c r="C110" s="7">
-        <v>1020</v>
+        <v>1009</v>
       </c>
       <c r="D110" s="6"/>
       <c r="E110" s="7"/>
@@ -1867,7 +1861,7 @@
         <v>0</v>
       </c>
       <c r="C111" s="7">
-        <v>1026</v>
+        <v>1011</v>
       </c>
       <c r="D111" s="6"/>
       <c r="E111" s="7"/>
@@ -1880,7 +1874,7 @@
         <v>0</v>
       </c>
       <c r="C112" s="7">
-        <v>1027</v>
+        <v>1013</v>
       </c>
       <c r="D112" s="6"/>
       <c r="E112" s="7"/>
@@ -1893,7 +1887,7 @@
         <v>0</v>
       </c>
       <c r="C113" s="7">
-        <v>1028</v>
+        <v>1020</v>
       </c>
       <c r="D113" s="6"/>
       <c r="E113" s="7"/>
@@ -1906,7 +1900,7 @@
         <v>0</v>
       </c>
       <c r="C114" s="7">
-        <v>1029</v>
+        <v>1026</v>
       </c>
       <c r="D114" s="6"/>
       <c r="E114" s="7"/>
@@ -1919,7 +1913,7 @@
         <v>0</v>
       </c>
       <c r="C115" s="7">
-        <v>1030</v>
+        <v>1027</v>
       </c>
       <c r="D115" s="6"/>
       <c r="E115" s="7"/>
@@ -1932,7 +1926,7 @@
         <v>0</v>
       </c>
       <c r="C116" s="7">
-        <v>1031</v>
+        <v>1028</v>
       </c>
       <c r="D116" s="6"/>
       <c r="E116" s="7"/>
@@ -1945,8 +1939,9 @@
         <v>0</v>
       </c>
       <c r="C117" s="7">
-        <v>1081</v>
-      </c>
+        <v>1029</v>
+      </c>
+      <c r="D117" s="6"/>
       <c r="E117" s="7"/>
     </row>
     <row r="118" spans="1:5">
@@ -1957,7 +1952,7 @@
         <v>0</v>
       </c>
       <c r="C118" s="7">
-        <v>1083</v>
+        <v>1030</v>
       </c>
       <c r="D118" s="6"/>
       <c r="E118" s="7"/>
@@ -1970,54 +1965,47 @@
         <v>0</v>
       </c>
       <c r="C119" s="7">
-        <v>1087</v>
+        <v>1031</v>
       </c>
       <c r="D119" s="6"/>
       <c r="E119" s="7"/>
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B120" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C120" s="7">
-        <v>748</v>
-      </c>
-      <c r="D120" s="6">
-        <v>757</v>
+        <v>1081</v>
       </c>
       <c r="E120" s="7"/>
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B121" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C121" s="7">
-        <v>748</v>
-      </c>
-      <c r="D121" s="6">
-        <v>759</v>
-      </c>
+        <v>1083</v>
+      </c>
+      <c r="D121" s="6"/>
       <c r="E121" s="7"/>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B122" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C122" s="7">
-        <v>748</v>
-      </c>
-      <c r="D122" s="6">
-        <v>760</v>
-      </c>
+        <v>1087</v>
+      </c>
+      <c r="D122" s="6"/>
       <c r="E122" s="7"/>
     </row>
     <row r="123" spans="1:5">
@@ -2028,7 +2016,7 @@
         <v>0</v>
       </c>
       <c r="C123" s="7">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="D123" s="6">
         <v>757</v>
@@ -2043,7 +2031,7 @@
         <v>0</v>
       </c>
       <c r="C124" s="7">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="D124" s="6">
         <v>759</v>
@@ -2058,7 +2046,7 @@
         <v>0</v>
       </c>
       <c r="C125" s="7">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="D125" s="6">
         <v>760</v>
@@ -2073,7 +2061,7 @@
         <v>0</v>
       </c>
       <c r="C126" s="7">
-        <v>775</v>
+        <v>749</v>
       </c>
       <c r="D126" s="6">
         <v>757</v>
@@ -2088,7 +2076,7 @@
         <v>0</v>
       </c>
       <c r="C127" s="7">
-        <v>775</v>
+        <v>749</v>
       </c>
       <c r="D127" s="6">
         <v>759</v>
@@ -2103,7 +2091,7 @@
         <v>0</v>
       </c>
       <c r="C128" s="7">
-        <v>775</v>
+        <v>749</v>
       </c>
       <c r="D128" s="6">
         <v>760</v>
@@ -2115,13 +2103,13 @@
         <v>5</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C129" s="7">
-        <v>761</v>
+        <v>775</v>
       </c>
       <c r="D129" s="6">
-        <v>762</v>
+        <v>757</v>
       </c>
       <c r="E129" s="7"/>
     </row>
@@ -2130,13 +2118,13 @@
         <v>5</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C130" s="7">
-        <v>761</v>
+        <v>775</v>
       </c>
       <c r="D130" s="6">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="E130" s="7"/>
     </row>
@@ -2145,13 +2133,13 @@
         <v>5</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C131" s="7">
-        <v>761</v>
+        <v>775</v>
       </c>
       <c r="D131" s="6">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="E131" s="7"/>
     </row>
@@ -2160,13 +2148,13 @@
         <v>5</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C132" s="7">
-        <v>746</v>
+        <v>761</v>
       </c>
       <c r="D132" s="6">
-        <v>783</v>
+        <v>762</v>
       </c>
       <c r="E132" s="7"/>
     </row>
@@ -2175,13 +2163,13 @@
         <v>5</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C133" s="7">
-        <v>746</v>
+        <v>761</v>
       </c>
       <c r="D133" s="6">
-        <v>784</v>
+        <v>763</v>
       </c>
       <c r="E133" s="7"/>
     </row>
@@ -2190,13 +2178,13 @@
         <v>5</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C134" s="8">
-        <v>746</v>
-      </c>
-      <c r="D134" s="8">
-        <v>746</v>
+        <v>1</v>
+      </c>
+      <c r="C134" s="7">
+        <v>761</v>
+      </c>
+      <c r="D134" s="6">
+        <v>764</v>
       </c>
       <c r="E134" s="7"/>
     </row>
@@ -2205,13 +2193,13 @@
         <v>5</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C135" s="8">
-        <v>747</v>
-      </c>
-      <c r="D135" s="8">
-        <v>747</v>
+        <v>2</v>
+      </c>
+      <c r="C135" s="7">
+        <v>782</v>
+      </c>
+      <c r="D135" s="6">
+        <v>783</v>
       </c>
       <c r="E135" s="7"/>
     </row>
@@ -2220,13 +2208,11 @@
         <v>5</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C136" s="8">
-        <v>750</v>
-      </c>
-      <c r="D136" s="8">
-        <v>750</v>
+        <v>2</v>
+      </c>
+      <c r="C136" s="7"/>
+      <c r="D136" s="6">
+        <v>784</v>
       </c>
       <c r="E136" s="7"/>
     </row>
@@ -2237,11 +2223,11 @@
       <c r="B137" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C137" s="8">
-        <v>751</v>
+      <c r="C137" s="7">
+        <v>782</v>
       </c>
       <c r="D137" s="8">
-        <v>751</v>
+        <v>782</v>
       </c>
       <c r="E137" s="7"/>
     </row>
@@ -2250,13 +2236,13 @@
         <v>5</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C138" s="7">
-        <v>748</v>
-      </c>
-      <c r="D138" s="6">
-        <v>1073</v>
+        <v>3</v>
+      </c>
+      <c r="C138" s="8">
+        <v>747</v>
+      </c>
+      <c r="D138" s="8">
+        <v>747</v>
       </c>
       <c r="E138" s="7"/>
     </row>
@@ -2265,13 +2251,13 @@
         <v>5</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C139" s="7">
-        <v>749</v>
-      </c>
-      <c r="D139" s="6">
-        <v>1074</v>
+        <v>3</v>
+      </c>
+      <c r="C139" s="8">
+        <v>750</v>
+      </c>
+      <c r="D139" s="8">
+        <v>750</v>
       </c>
       <c r="E139" s="7"/>
     </row>
@@ -2280,13 +2266,13 @@
         <v>5</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C140" s="7">
-        <v>858</v>
-      </c>
-      <c r="D140" s="9">
-        <v>965</v>
+        <v>3</v>
+      </c>
+      <c r="C140" s="8">
+        <v>751</v>
+      </c>
+      <c r="D140" s="8">
+        <v>751</v>
       </c>
       <c r="E140" s="7"/>
     </row>
@@ -2298,10 +2284,10 @@
         <v>4</v>
       </c>
       <c r="C141" s="7">
-        <v>859</v>
-      </c>
-      <c r="D141" s="9">
-        <v>967</v>
+        <v>748</v>
+      </c>
+      <c r="D141" s="6">
+        <v>1073</v>
       </c>
       <c r="E141" s="7"/>
     </row>
@@ -2312,10 +2298,12 @@
       <c r="B142" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C142" s="2">
-        <v>860</v>
-      </c>
-      <c r="D142" s="6"/>
+      <c r="C142" s="7">
+        <v>749</v>
+      </c>
+      <c r="D142" s="6">
+        <v>1074</v>
+      </c>
       <c r="E142" s="7"/>
     </row>
     <row r="143" spans="1:5">
@@ -2325,17 +2313,60 @@
       <c r="B143" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C143" s="3">
+      <c r="C143" s="7">
+        <v>858</v>
+      </c>
+      <c r="D143" s="9">
+        <v>965</v>
+      </c>
+      <c r="E143" s="7"/>
+    </row>
+    <row r="144" spans="1:5">
+      <c r="A144" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B144" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C144" s="7">
+        <v>859</v>
+      </c>
+      <c r="D144" s="9">
+        <v>967</v>
+      </c>
+      <c r="E144" s="7"/>
+    </row>
+    <row r="145" spans="1:5">
+      <c r="A145" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B145" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C145" s="2">
+        <v>860</v>
+      </c>
+      <c r="D145" s="6"/>
+      <c r="E145" s="7"/>
+    </row>
+    <row r="146" spans="1:5">
+      <c r="A146" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B146" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C146" s="3">
         <v>1013</v>
       </c>
-      <c r="D143" s="6"/>
-      <c r="E143" s="7"/>
-    </row>
-    <row r="144" spans="1:5">
-      <c r="E144" s="7"/>
+      <c r="D146" s="6"/>
+      <c r="E146" s="7"/>
+    </row>
+    <row r="147" spans="1:5">
+      <c r="E147" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D143">
+  <autoFilter ref="A1:D146">
     <sortState ref="A2:D147">
       <sortCondition ref="A2:A147"/>
       <sortCondition ref="B2:B147"/>

</xml_diff>